<commit_message>
Updates for default, test script
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_input.xlsx
+++ b/applications/default/data/national/default_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F6C21532-67B1-FA46-ABBB-7C586B3E11A9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{518C0E23-D2C4-B344-9720-3F3088D82331}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="-20740" windowWidth="27100" windowHeight="18820" tabRatio="961" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="-20740" windowWidth="27100" windowHeight="18820" tabRatio="961" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -2346,10 +2346,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2430,6 +2426,10 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="727">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -4600,10 +4600,10 @@
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="64" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4765,7 +4765,7 @@
       <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="66" t="s">
         <v>104</v>
       </c>
       <c r="C25" s="25">
@@ -4809,7 +4809,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="66" t="s">
         <v>105</v>
       </c>
       <c r="C30" s="25">
@@ -4973,201 +4973,201 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="56" style="82" customWidth="1"/>
-    <col min="2" max="2" width="20" style="61" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="60" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="60" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="60"/>
+    <col min="1" max="1" width="56" style="80" customWidth="1"/>
+    <col min="2" max="2" width="20" style="59" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="58" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" style="58" customWidth="1"/>
+    <col min="5" max="16384" width="14.5" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="90" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="89" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="88" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="83">
-        <v>0</v>
-      </c>
-      <c r="C2" s="83">
+      <c r="B2" s="81">
+        <v>0</v>
+      </c>
+      <c r="C2" s="81">
         <v>0.95</v>
       </c>
-      <c r="D2" s="84">
+      <c r="D2" s="82">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="83">
-        <v>0</v>
-      </c>
-      <c r="C3" s="83">
+      <c r="B3" s="81">
+        <v>0</v>
+      </c>
+      <c r="C3" s="81">
         <v>0.95</v>
       </c>
-      <c r="D3" s="84">
+      <c r="D3" s="82">
         <v>0.8</v>
       </c>
-      <c r="E3" s="89"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="83">
-        <v>0</v>
-      </c>
-      <c r="C4" s="83">
+      <c r="B4" s="81">
+        <v>0</v>
+      </c>
+      <c r="C4" s="81">
         <v>0.95</v>
       </c>
-      <c r="D4" s="84">
-        <v>1</v>
-      </c>
-      <c r="E4" s="69"/>
+      <c r="D4" s="82">
+        <v>1</v>
+      </c>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="81">
         <v>0.1</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="81">
         <v>0.95</v>
       </c>
-      <c r="D5" s="84">
+      <c r="D5" s="82">
         <f>180</f>
         <v>180</v>
       </c>
-      <c r="E5" s="69"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="83">
+      <c r="B6" s="81">
         <v>0.5</v>
       </c>
-      <c r="C6" s="83">
+      <c r="C6" s="81">
         <v>0.95</v>
       </c>
-      <c r="D6" s="85">
+      <c r="D6" s="83">
         <f>SUM('Programs family planning'!E2:E10)</f>
         <v>0.82100000000000006</v>
       </c>
-      <c r="E6" s="88"/>
+      <c r="E6" s="86"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="83">
-        <v>0</v>
-      </c>
-      <c r="C7" s="83">
+      <c r="B7" s="81">
+        <v>0</v>
+      </c>
+      <c r="C7" s="81">
         <v>0.95</v>
       </c>
-      <c r="D7" s="84">
+      <c r="D7" s="82">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E7" s="87"/>
+      <c r="E7" s="85"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="83">
-        <v>0</v>
-      </c>
-      <c r="C8" s="83">
+      <c r="B8" s="81">
+        <v>0</v>
+      </c>
+      <c r="C8" s="81">
         <v>0.95</v>
       </c>
-      <c r="D8" s="84">
+      <c r="D8" s="82">
         <v>0.75</v>
       </c>
-      <c r="E8" s="87"/>
+      <c r="E8" s="85"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="83">
-        <v>0</v>
-      </c>
-      <c r="C9" s="83">
+      <c r="B9" s="81">
+        <v>0</v>
+      </c>
+      <c r="C9" s="81">
         <v>0.95</v>
       </c>
-      <c r="D9" s="84">
+      <c r="D9" s="82">
         <v>0.19</v>
       </c>
-      <c r="E9" s="87"/>
+      <c r="E9" s="85"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="101" t="s">
         <v>218</v>
       </c>
-      <c r="B10" s="83">
-        <v>0</v>
-      </c>
-      <c r="C10" s="83">
+      <c r="B10" s="81">
+        <v>0</v>
+      </c>
+      <c r="C10" s="81">
         <v>0.95</v>
       </c>
-      <c r="D10" s="84">
+      <c r="D10" s="82">
         <v>0.73</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="101" t="s">
         <v>219</v>
       </c>
-      <c r="B11" s="83">
-        <v>0</v>
-      </c>
-      <c r="C11" s="83">
+      <c r="B11" s="81">
+        <v>0</v>
+      </c>
+      <c r="C11" s="81">
         <v>0.95</v>
       </c>
-      <c r="D11" s="84">
+      <c r="D11" s="82">
         <v>1.78</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="101" t="s">
         <v>220</v>
       </c>
-      <c r="B12" s="83">
-        <v>0</v>
-      </c>
-      <c r="C12" s="83">
+      <c r="B12" s="81">
+        <v>0</v>
+      </c>
+      <c r="C12" s="81">
         <v>0.95</v>
       </c>
-      <c r="D12" s="84">
+      <c r="D12" s="82">
         <v>0.24</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="B13" s="83">
-        <v>0</v>
-      </c>
-      <c r="C13" s="83">
+      <c r="B13" s="81">
+        <v>0</v>
+      </c>
+      <c r="C13" s="81">
         <v>0.95</v>
       </c>
-      <c r="D13" s="84">
+      <c r="D13" s="82">
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -5175,13 +5175,13 @@
       <c r="A14" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="B14" s="83">
-        <v>0</v>
-      </c>
-      <c r="C14" s="83">
+      <c r="B14" s="81">
+        <v>0</v>
+      </c>
+      <c r="C14" s="81">
         <v>0.95</v>
       </c>
-      <c r="D14" s="84">
+      <c r="D14" s="82">
         <v>0.73</v>
       </c>
     </row>
@@ -5189,339 +5189,339 @@
       <c r="A15" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="B15" s="83">
-        <v>0</v>
-      </c>
-      <c r="C15" s="83">
+      <c r="B15" s="81">
+        <v>0</v>
+      </c>
+      <c r="C15" s="81">
         <v>0.95</v>
       </c>
-      <c r="D15" s="84">
+      <c r="D15" s="82">
         <v>1.78</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="83">
-        <v>0</v>
-      </c>
-      <c r="C16" s="83">
+      <c r="B16" s="81">
+        <v>0</v>
+      </c>
+      <c r="C16" s="81">
         <v>0.95</v>
       </c>
-      <c r="D16" s="84">
+      <c r="D16" s="82">
         <v>2.06</v>
       </c>
-      <c r="E16" s="69"/>
+      <c r="E16" s="67"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="83">
-        <v>0</v>
-      </c>
-      <c r="C17" s="83">
+      <c r="B17" s="81">
+        <v>0</v>
+      </c>
+      <c r="C17" s="81">
         <v>0.95</v>
       </c>
-      <c r="D17" s="84">
+      <c r="D17" s="82">
         <v>0.25</v>
       </c>
-      <c r="E17" s="69"/>
+      <c r="E17" s="67"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="82" t="s">
+      <c r="A18" s="80" t="s">
         <v>199</v>
       </c>
-      <c r="B18" s="83">
-        <v>0</v>
-      </c>
-      <c r="C18" s="83">
+      <c r="B18" s="81">
+        <v>0</v>
+      </c>
+      <c r="C18" s="81">
         <v>0.95</v>
       </c>
-      <c r="D18" s="102">
+      <c r="D18" s="100">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
         <v>1.22</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="80" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="83">
-        <v>0</v>
-      </c>
-      <c r="C19" s="83">
+      <c r="B19" s="81">
+        <v>0</v>
+      </c>
+      <c r="C19" s="81">
         <v>0.95</v>
       </c>
-      <c r="D19" s="102">
+      <c r="D19" s="100">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
         <v>1.4700000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="82" t="s">
+      <c r="A20" s="80" t="s">
         <v>196</v>
       </c>
-      <c r="B20" s="83">
-        <v>0</v>
-      </c>
-      <c r="C20" s="83">
+      <c r="B20" s="81">
+        <v>0</v>
+      </c>
+      <c r="C20" s="81">
         <v>0.95</v>
       </c>
-      <c r="D20" s="102">
+      <c r="D20" s="100">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$16:$E$20&lt;&gt;""))</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="82" t="s">
+      <c r="A21" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="83">
-        <v>0</v>
-      </c>
-      <c r="C21" s="83">
+      <c r="B21" s="81">
+        <v>0</v>
+      </c>
+      <c r="C21" s="81">
         <v>0.95</v>
       </c>
-      <c r="D21" s="84">
+      <c r="D21" s="82">
         <v>50</v>
       </c>
-      <c r="E21" s="69"/>
+      <c r="E21" s="67"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="83">
+      <c r="B22" s="81">
         <v>0.2</v>
       </c>
-      <c r="C22" s="83">
+      <c r="C22" s="81">
         <v>0.95</v>
       </c>
-      <c r="D22" s="84">
+      <c r="D22" s="82">
         <v>2.61</v>
       </c>
-      <c r="E22" s="69"/>
+      <c r="E22" s="67"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="82" t="s">
+      <c r="A23" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="83">
-        <v>0</v>
-      </c>
-      <c r="C23" s="83">
+      <c r="B23" s="81">
+        <v>0</v>
+      </c>
+      <c r="C23" s="81">
         <v>0.95</v>
       </c>
-      <c r="D23" s="84">
-        <v>1</v>
-      </c>
-      <c r="E23" s="69"/>
+      <c r="D23" s="82">
+        <v>1</v>
+      </c>
+      <c r="E23" s="67"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="83">
-        <v>0</v>
-      </c>
-      <c r="C24" s="83">
+      <c r="B24" s="81">
+        <v>0</v>
+      </c>
+      <c r="C24" s="81">
         <v>0.95</v>
       </c>
-      <c r="D24" s="84">
-        <v>1</v>
-      </c>
-      <c r="E24" s="86"/>
+      <c r="D24" s="82">
+        <v>1</v>
+      </c>
+      <c r="E24" s="84"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="82" t="s">
+      <c r="A25" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="B25" s="83">
-        <v>0</v>
-      </c>
-      <c r="C25" s="83">
+      <c r="B25" s="81">
+        <v>0</v>
+      </c>
+      <c r="C25" s="81">
         <v>0.95</v>
       </c>
-      <c r="D25" s="84">
-        <v>1</v>
-      </c>
-      <c r="E25" s="69"/>
+      <c r="D25" s="82">
+        <v>1</v>
+      </c>
+      <c r="E25" s="67"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="83">
-        <v>0</v>
-      </c>
-      <c r="C26" s="83">
+      <c r="B26" s="81">
+        <v>0</v>
+      </c>
+      <c r="C26" s="81">
         <v>0.95</v>
       </c>
-      <c r="D26" s="84">
+      <c r="D26" s="82">
         <v>2.99</v>
       </c>
-      <c r="E26" s="69"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="83">
-        <v>0</v>
-      </c>
-      <c r="C27" s="83">
+      <c r="B27" s="81">
+        <v>0</v>
+      </c>
+      <c r="C27" s="81">
         <v>0.95</v>
       </c>
-      <c r="D27" s="84">
+      <c r="D27" s="82">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="83">
-        <v>0</v>
-      </c>
-      <c r="C28" s="83">
+      <c r="B28" s="81">
+        <v>0</v>
+      </c>
+      <c r="C28" s="81">
         <v>0.95</v>
       </c>
-      <c r="D28" s="84">
+      <c r="D28" s="82">
         <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="82" t="s">
+      <c r="A29" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="83">
-        <v>0</v>
-      </c>
-      <c r="C29" s="83">
+      <c r="B29" s="81">
+        <v>0</v>
+      </c>
+      <c r="C29" s="81">
         <v>0.95</v>
       </c>
-      <c r="D29" s="85">
+      <c r="D29" s="83">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
         <v>23.363600000000005</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="82" t="s">
+      <c r="A30" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="83">
-        <v>0</v>
-      </c>
-      <c r="C30" s="83">
+      <c r="B30" s="81">
+        <v>0</v>
+      </c>
+      <c r="C30" s="81">
         <v>0.95</v>
       </c>
-      <c r="D30" s="84">
+      <c r="D30" s="82">
         <v>0.35</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="82" t="s">
+      <c r="A31" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="83">
-        <v>0</v>
-      </c>
-      <c r="C31" s="83">
+      <c r="B31" s="81">
+        <v>0</v>
+      </c>
+      <c r="C31" s="81">
         <v>0.95</v>
       </c>
-      <c r="D31" s="84">
+      <c r="D31" s="82">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="83">
-        <v>0</v>
-      </c>
-      <c r="C32" s="83">
+      <c r="B32" s="81">
+        <v>0</v>
+      </c>
+      <c r="C32" s="81">
         <v>0.95</v>
       </c>
-      <c r="D32" s="84">
+      <c r="D32" s="82">
         <v>2.8</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="83">
-        <v>0</v>
-      </c>
-      <c r="C33" s="83">
+      <c r="B33" s="81">
+        <v>0</v>
+      </c>
+      <c r="C33" s="81">
         <v>0.95</v>
       </c>
-      <c r="D33" s="84">
+      <c r="D33" s="82">
         <v>50.26</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="82" t="s">
+      <c r="A34" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="83">
-        <v>0</v>
-      </c>
-      <c r="C34" s="83">
+      <c r="B34" s="81">
+        <v>0</v>
+      </c>
+      <c r="C34" s="81">
         <v>0.95</v>
       </c>
-      <c r="D34" s="84">
+      <c r="D34" s="82">
         <v>36.1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="82" t="s">
+    <row r="35" spans="1:6" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="83">
-        <v>0</v>
-      </c>
-      <c r="C35" s="83">
+      <c r="B35" s="81">
+        <v>0</v>
+      </c>
+      <c r="C35" s="81">
         <v>0.95</v>
       </c>
-      <c r="D35" s="84">
+      <c r="D35" s="82">
         <v>231.85</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="58"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="82" t="s">
+      <c r="A36" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="83">
-        <v>0</v>
-      </c>
-      <c r="C36" s="83">
+      <c r="B36" s="81">
+        <v>0</v>
+      </c>
+      <c r="C36" s="81">
         <v>0.95</v>
       </c>
-      <c r="D36" s="84">
+      <c r="D36" s="82">
         <v>1.5</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="82" t="s">
+      <c r="A37" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="83">
-        <v>0</v>
-      </c>
-      <c r="C37" s="83">
+      <c r="B37" s="81">
+        <v>0</v>
+      </c>
+      <c r="C37" s="81">
         <v>0.95</v>
       </c>
-      <c r="D37" s="84">
+      <c r="D37" s="82">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F38" s="61"/>
+      <c r="F38" s="59"/>
     </row>
   </sheetData>
   <sortState ref="A2:D37">
@@ -5546,116 +5546,116 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="93" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="93"/>
+    <col min="1" max="1" width="18.6640625" style="91" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="91"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="96" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="95" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="95" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="94" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="84">
+      <c r="C2" s="82">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D2" s="84">
+      <c r="D2" s="82">
         <f>0.5*0.61</f>
         <v>0.30499999999999999</v>
       </c>
-      <c r="E2" s="84">
+      <c r="E2" s="82">
         <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="84">
+      <c r="A3" s="93"/>
+      <c r="B3" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="82">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D3" s="84">
+      <c r="D3" s="82">
         <f>0.5*0.61</f>
         <v>0.30499999999999999</v>
       </c>
-      <c r="E3" s="84">
+      <c r="E3" s="82">
         <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="95"/>
-      <c r="B4" s="95" t="s">
+      <c r="A4" s="93"/>
+      <c r="B4" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="84">
+      <c r="C4" s="82">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D4" s="84">
+      <c r="D4" s="82">
         <f>0.5*0.61</f>
         <v>0.30499999999999999</v>
       </c>
-      <c r="E4" s="84">
+      <c r="E4" s="82">
         <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="95"/>
-      <c r="B5" s="95" t="s">
+      <c r="A5" s="93"/>
+      <c r="B5" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="82">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D5" s="84">
+      <c r="D5" s="82">
         <f>0.5*0.61</f>
         <v>0.30499999999999999</v>
       </c>
-      <c r="E5" s="84">
+      <c r="E5" s="82">
         <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="95"/>
-      <c r="B6" s="95" t="s">
+      <c r="A6" s="93"/>
+      <c r="B6" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="84">
+      <c r="C6" s="82">
         <f>1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D6" s="84">
+      <c r="D6" s="82">
         <f>0.5*0.61</f>
         <v>0.30499999999999999</v>
       </c>
-      <c r="E6" s="84">
+      <c r="E6" s="82">
         <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="94"/>
+      <c r="C9" s="92"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5676,20 +5676,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="53" style="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="60" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="60"/>
+    <col min="1" max="1" width="53" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="58" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="63" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="63" t="s">
         <v>209</v>
       </c>
     </row>
@@ -5697,37 +5697,37 @@
       <c r="A2" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="74"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="76"/>
+      <c r="C3" s="74"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="C5" s="76"/>
+      <c r="C5" s="74"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="52"/>
@@ -5773,84 +5773,84 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="60" customWidth="1"/>
-    <col min="2" max="16384" width="11.5" style="60"/>
+    <col min="1" max="1" width="30.1640625" style="58" customWidth="1"/>
+    <col min="2" max="16384" width="11.5" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="74" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="74" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="74" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="74" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="74" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="74" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="74" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="76"/>
+      <c r="A10" s="74"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="76"/>
+      <c r="A11" s="74"/>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="76"/>
+      <c r="A12" s="74"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="76"/>
+      <c r="A13" s="74"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="76"/>
+      <c r="A14" s="74"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A15" s="76"/>
+      <c r="A15" s="74"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A16" s="76"/>
+      <c r="A16" s="74"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="76"/>
+      <c r="A17" s="74"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="76"/>
+      <c r="A18" s="74"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="76"/>
+      <c r="A19" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6050,47 +6050,47 @@
       <c r="B2" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="56">
-        <v>0</v>
-      </c>
-      <c r="D2" s="56">
+      <c r="C2" s="54">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="E2" s="56">
+      <c r="E2" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="F2" s="56">
+      <c r="F2" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="G2" s="56">
+      <c r="G2" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="H2" s="57">
-        <v>0</v>
-      </c>
-      <c r="I2" s="57">
-        <v>0</v>
-      </c>
-      <c r="J2" s="57">
-        <v>0</v>
-      </c>
-      <c r="K2" s="57">
-        <v>0</v>
-      </c>
-      <c r="L2" s="57">
-        <v>0</v>
-      </c>
-      <c r="M2" s="57">
-        <v>0</v>
-      </c>
-      <c r="N2" s="57">
-        <v>0</v>
-      </c>
-      <c r="O2" s="57">
+      <c r="H2" s="55">
+        <v>0</v>
+      </c>
+      <c r="I2" s="55">
+        <v>0</v>
+      </c>
+      <c r="J2" s="55">
+        <v>0</v>
+      </c>
+      <c r="K2" s="55">
+        <v>0</v>
+      </c>
+      <c r="L2" s="55">
+        <v>0</v>
+      </c>
+      <c r="M2" s="55">
+        <v>0</v>
+      </c>
+      <c r="N2" s="55">
+        <v>0</v>
+      </c>
+      <c r="O2" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6098,43 +6098,43 @@
       <c r="B3" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="59">
-        <v>1</v>
-      </c>
-      <c r="D3" s="56">
-        <v>0</v>
-      </c>
-      <c r="E3" s="56">
-        <v>0</v>
-      </c>
-      <c r="F3" s="56">
-        <v>0</v>
-      </c>
-      <c r="G3" s="56">
-        <v>0</v>
-      </c>
-      <c r="H3" s="57">
-        <v>0</v>
-      </c>
-      <c r="I3" s="57">
-        <v>0</v>
-      </c>
-      <c r="J3" s="57">
-        <v>0</v>
-      </c>
-      <c r="K3" s="57">
-        <v>0</v>
-      </c>
-      <c r="L3" s="57">
-        <v>0</v>
-      </c>
-      <c r="M3" s="57">
-        <v>0</v>
-      </c>
-      <c r="N3" s="57">
-        <v>0</v>
-      </c>
-      <c r="O3" s="57">
+      <c r="C3" s="57">
+        <v>1</v>
+      </c>
+      <c r="D3" s="54">
+        <v>0</v>
+      </c>
+      <c r="E3" s="54">
+        <v>0</v>
+      </c>
+      <c r="F3" s="54">
+        <v>0</v>
+      </c>
+      <c r="G3" s="54">
+        <v>0</v>
+      </c>
+      <c r="H3" s="55">
+        <v>0</v>
+      </c>
+      <c r="I3" s="55">
+        <v>0</v>
+      </c>
+      <c r="J3" s="55">
+        <v>0</v>
+      </c>
+      <c r="K3" s="55">
+        <v>0</v>
+      </c>
+      <c r="L3" s="55">
+        <v>0</v>
+      </c>
+      <c r="M3" s="55">
+        <v>0</v>
+      </c>
+      <c r="N3" s="55">
+        <v>0</v>
+      </c>
+      <c r="O3" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6142,45 +6142,45 @@
       <c r="B4" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="56">
-        <v>0</v>
-      </c>
-      <c r="D4" s="56">
-        <v>0</v>
-      </c>
-      <c r="E4" s="56">
+      <c r="C4" s="54">
+        <v>0</v>
+      </c>
+      <c r="D4" s="54">
+        <v>0</v>
+      </c>
+      <c r="E4" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="F4" s="56">
+      <c r="F4" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="G4" s="56">
-        <v>0</v>
-      </c>
-      <c r="H4" s="57">
-        <v>0</v>
-      </c>
-      <c r="I4" s="57">
-        <v>0</v>
-      </c>
-      <c r="J4" s="57">
-        <v>0</v>
-      </c>
-      <c r="K4" s="57">
-        <v>0</v>
-      </c>
-      <c r="L4" s="57">
-        <v>0</v>
-      </c>
-      <c r="M4" s="57">
-        <v>0</v>
-      </c>
-      <c r="N4" s="57">
-        <v>0</v>
-      </c>
-      <c r="O4" s="57">
+      <c r="G4" s="54">
+        <v>0</v>
+      </c>
+      <c r="H4" s="55">
+        <v>0</v>
+      </c>
+      <c r="I4" s="55">
+        <v>0</v>
+      </c>
+      <c r="J4" s="55">
+        <v>0</v>
+      </c>
+      <c r="K4" s="55">
+        <v>0</v>
+      </c>
+      <c r="L4" s="55">
+        <v>0</v>
+      </c>
+      <c r="M4" s="55">
+        <v>0</v>
+      </c>
+      <c r="N4" s="55">
+        <v>0</v>
+      </c>
+      <c r="O4" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6188,46 +6188,46 @@
       <c r="B5" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="56">
-        <v>0</v>
-      </c>
-      <c r="D5" s="56">
-        <v>0</v>
-      </c>
-      <c r="E5" s="56">
+      <c r="C5" s="54">
+        <v>0</v>
+      </c>
+      <c r="D5" s="54">
+        <v>0</v>
+      </c>
+      <c r="E5" s="54">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="F5" s="56">
+      <c r="F5" s="54">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="G5" s="56">
+      <c r="G5" s="54">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="H5" s="57">
-        <v>0</v>
-      </c>
-      <c r="I5" s="57">
-        <v>0</v>
-      </c>
-      <c r="J5" s="57">
-        <v>0</v>
-      </c>
-      <c r="K5" s="57">
-        <v>0</v>
-      </c>
-      <c r="L5" s="57">
-        <v>0</v>
-      </c>
-      <c r="M5" s="57">
-        <v>0</v>
-      </c>
-      <c r="N5" s="57">
-        <v>0</v>
-      </c>
-      <c r="O5" s="57">
+      <c r="H5" s="55">
+        <v>0</v>
+      </c>
+      <c r="I5" s="55">
+        <v>0</v>
+      </c>
+      <c r="J5" s="55">
+        <v>0</v>
+      </c>
+      <c r="K5" s="55">
+        <v>0</v>
+      </c>
+      <c r="L5" s="55">
+        <v>0</v>
+      </c>
+      <c r="M5" s="55">
+        <v>0</v>
+      </c>
+      <c r="N5" s="55">
+        <v>0</v>
+      </c>
+      <c r="O5" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6235,43 +6235,43 @@
       <c r="B6" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="56">
-        <v>1</v>
-      </c>
-      <c r="D6" s="56">
-        <v>1</v>
-      </c>
-      <c r="E6" s="56">
-        <v>1</v>
-      </c>
-      <c r="F6" s="56">
-        <v>1</v>
-      </c>
-      <c r="G6" s="56">
-        <v>1</v>
-      </c>
-      <c r="H6" s="57">
-        <v>0</v>
-      </c>
-      <c r="I6" s="57">
-        <v>0</v>
-      </c>
-      <c r="J6" s="57">
-        <v>0</v>
-      </c>
-      <c r="K6" s="57">
-        <v>0</v>
-      </c>
-      <c r="L6" s="57">
-        <v>0</v>
-      </c>
-      <c r="M6" s="57">
-        <v>0</v>
-      </c>
-      <c r="N6" s="57">
-        <v>0</v>
-      </c>
-      <c r="O6" s="57">
+      <c r="C6" s="54">
+        <v>1</v>
+      </c>
+      <c r="D6" s="54">
+        <v>1</v>
+      </c>
+      <c r="E6" s="54">
+        <v>1</v>
+      </c>
+      <c r="F6" s="54">
+        <v>1</v>
+      </c>
+      <c r="G6" s="54">
+        <v>1</v>
+      </c>
+      <c r="H6" s="55">
+        <v>0</v>
+      </c>
+      <c r="I6" s="55">
+        <v>0</v>
+      </c>
+      <c r="J6" s="55">
+        <v>0</v>
+      </c>
+      <c r="K6" s="55">
+        <v>0</v>
+      </c>
+      <c r="L6" s="55">
+        <v>0</v>
+      </c>
+      <c r="M6" s="55">
+        <v>0</v>
+      </c>
+      <c r="N6" s="55">
+        <v>0</v>
+      </c>
+      <c r="O6" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6279,45 +6279,45 @@
       <c r="B7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="56">
-        <v>0</v>
-      </c>
-      <c r="D7" s="56">
-        <v>0</v>
-      </c>
-      <c r="E7" s="56">
+      <c r="C7" s="54">
+        <v>0</v>
+      </c>
+      <c r="D7" s="54">
+        <v>0</v>
+      </c>
+      <c r="E7" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="F7" s="56">
+      <c r="F7" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="G7" s="56">
-        <v>0</v>
-      </c>
-      <c r="H7" s="57">
-        <v>0</v>
-      </c>
-      <c r="I7" s="57">
-        <v>0</v>
-      </c>
-      <c r="J7" s="57">
-        <v>0</v>
-      </c>
-      <c r="K7" s="57">
-        <v>0</v>
-      </c>
-      <c r="L7" s="57">
-        <v>0</v>
-      </c>
-      <c r="M7" s="57">
-        <v>0</v>
-      </c>
-      <c r="N7" s="57">
-        <v>0</v>
-      </c>
-      <c r="O7" s="57">
+      <c r="G7" s="54">
+        <v>0</v>
+      </c>
+      <c r="H7" s="55">
+        <v>0</v>
+      </c>
+      <c r="I7" s="55">
+        <v>0</v>
+      </c>
+      <c r="J7" s="55">
+        <v>0</v>
+      </c>
+      <c r="K7" s="55">
+        <v>0</v>
+      </c>
+      <c r="L7" s="55">
+        <v>0</v>
+      </c>
+      <c r="M7" s="55">
+        <v>0</v>
+      </c>
+      <c r="N7" s="55">
+        <v>0</v>
+      </c>
+      <c r="O7" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6325,47 +6325,47 @@
       <c r="B8" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="56">
-        <v>0</v>
-      </c>
-      <c r="D8" s="56">
+      <c r="C8" s="54">
+        <v>0</v>
+      </c>
+      <c r="D8" s="54">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
         <v>1</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="54">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
         <v>1</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="54">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
         <v>1</v>
       </c>
-      <c r="G8" s="56">
+      <c r="G8" s="54">
         <f>IF(ISBLANK(comm_deliv), frac_children_health_facility,1)</f>
         <v>1</v>
       </c>
-      <c r="H8" s="57">
-        <v>0</v>
-      </c>
-      <c r="I8" s="57">
-        <v>0</v>
-      </c>
-      <c r="J8" s="57">
-        <v>0</v>
-      </c>
-      <c r="K8" s="57">
-        <v>0</v>
-      </c>
-      <c r="L8" s="57">
-        <v>0</v>
-      </c>
-      <c r="M8" s="57">
-        <v>0</v>
-      </c>
-      <c r="N8" s="57">
-        <v>0</v>
-      </c>
-      <c r="O8" s="57">
+      <c r="H8" s="55">
+        <v>0</v>
+      </c>
+      <c r="I8" s="55">
+        <v>0</v>
+      </c>
+      <c r="J8" s="55">
+        <v>0</v>
+      </c>
+      <c r="K8" s="55">
+        <v>0</v>
+      </c>
+      <c r="L8" s="55">
+        <v>0</v>
+      </c>
+      <c r="M8" s="55">
+        <v>0</v>
+      </c>
+      <c r="N8" s="55">
+        <v>0</v>
+      </c>
+      <c r="O8" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6373,43 +6373,43 @@
       <c r="B9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="56">
-        <v>0</v>
-      </c>
-      <c r="D9" s="56">
-        <v>0</v>
-      </c>
-      <c r="E9" s="56">
-        <v>1</v>
-      </c>
-      <c r="F9" s="56">
-        <v>1</v>
-      </c>
-      <c r="G9" s="56">
-        <v>1</v>
-      </c>
-      <c r="H9" s="57">
-        <v>0</v>
-      </c>
-      <c r="I9" s="57">
-        <v>0</v>
-      </c>
-      <c r="J9" s="57">
-        <v>0</v>
-      </c>
-      <c r="K9" s="57">
-        <v>0</v>
-      </c>
-      <c r="L9" s="57">
-        <v>0</v>
-      </c>
-      <c r="M9" s="57">
-        <v>0</v>
-      </c>
-      <c r="N9" s="57">
-        <v>0</v>
-      </c>
-      <c r="O9" s="57">
+      <c r="C9" s="54">
+        <v>0</v>
+      </c>
+      <c r="D9" s="54">
+        <v>0</v>
+      </c>
+      <c r="E9" s="54">
+        <v>1</v>
+      </c>
+      <c r="F9" s="54">
+        <v>1</v>
+      </c>
+      <c r="G9" s="54">
+        <v>1</v>
+      </c>
+      <c r="H9" s="55">
+        <v>0</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0</v>
+      </c>
+      <c r="J9" s="55">
+        <v>0</v>
+      </c>
+      <c r="K9" s="55">
+        <v>0</v>
+      </c>
+      <c r="L9" s="55">
+        <v>0</v>
+      </c>
+      <c r="M9" s="55">
+        <v>0</v>
+      </c>
+      <c r="N9" s="55">
+        <v>0</v>
+      </c>
+      <c r="O9" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6417,43 +6417,43 @@
       <c r="B10" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="56">
-        <v>1</v>
-      </c>
-      <c r="D10" s="56">
-        <v>1</v>
-      </c>
-      <c r="E10" s="56">
-        <v>1</v>
-      </c>
-      <c r="F10" s="56">
-        <v>1</v>
-      </c>
-      <c r="G10" s="56">
-        <v>1</v>
-      </c>
-      <c r="H10" s="57">
-        <v>0</v>
-      </c>
-      <c r="I10" s="57">
-        <v>0</v>
-      </c>
-      <c r="J10" s="57">
-        <v>0</v>
-      </c>
-      <c r="K10" s="57">
-        <v>0</v>
-      </c>
-      <c r="L10" s="57">
-        <v>0</v>
-      </c>
-      <c r="M10" s="57">
-        <v>0</v>
-      </c>
-      <c r="N10" s="57">
-        <v>0</v>
-      </c>
-      <c r="O10" s="57">
+      <c r="C10" s="54">
+        <v>1</v>
+      </c>
+      <c r="D10" s="54">
+        <v>1</v>
+      </c>
+      <c r="E10" s="54">
+        <v>1</v>
+      </c>
+      <c r="F10" s="54">
+        <v>1</v>
+      </c>
+      <c r="G10" s="54">
+        <v>1</v>
+      </c>
+      <c r="H10" s="55">
+        <v>0</v>
+      </c>
+      <c r="I10" s="55">
+        <v>0</v>
+      </c>
+      <c r="J10" s="55">
+        <v>0</v>
+      </c>
+      <c r="K10" s="55">
+        <v>0</v>
+      </c>
+      <c r="L10" s="55">
+        <v>0</v>
+      </c>
+      <c r="M10" s="55">
+        <v>0</v>
+      </c>
+      <c r="N10" s="55">
+        <v>0</v>
+      </c>
+      <c r="O10" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6461,43 +6461,43 @@
       <c r="B11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="56">
-        <v>0</v>
-      </c>
-      <c r="D11" s="56">
-        <v>0</v>
-      </c>
-      <c r="E11" s="56">
-        <v>1</v>
-      </c>
-      <c r="F11" s="56">
-        <v>1</v>
-      </c>
-      <c r="G11" s="56">
-        <v>1</v>
-      </c>
-      <c r="H11" s="57">
-        <v>0</v>
-      </c>
-      <c r="I11" s="57">
-        <v>0</v>
-      </c>
-      <c r="J11" s="57">
-        <v>0</v>
-      </c>
-      <c r="K11" s="57">
-        <v>0</v>
-      </c>
-      <c r="L11" s="57">
-        <v>0</v>
-      </c>
-      <c r="M11" s="57">
-        <v>0</v>
-      </c>
-      <c r="N11" s="57">
-        <v>0</v>
-      </c>
-      <c r="O11" s="57">
+      <c r="C11" s="54">
+        <v>0</v>
+      </c>
+      <c r="D11" s="54">
+        <v>0</v>
+      </c>
+      <c r="E11" s="54">
+        <v>1</v>
+      </c>
+      <c r="F11" s="54">
+        <v>1</v>
+      </c>
+      <c r="G11" s="54">
+        <v>1</v>
+      </c>
+      <c r="H11" s="55">
+        <v>0</v>
+      </c>
+      <c r="I11" s="55">
+        <v>0</v>
+      </c>
+      <c r="J11" s="55">
+        <v>0</v>
+      </c>
+      <c r="K11" s="55">
+        <v>0</v>
+      </c>
+      <c r="L11" s="55">
+        <v>0</v>
+      </c>
+      <c r="M11" s="55">
+        <v>0</v>
+      </c>
+      <c r="N11" s="55">
+        <v>0</v>
+      </c>
+      <c r="O11" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6511,47 +6511,47 @@
       <c r="B13" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="57">
-        <v>0</v>
-      </c>
-      <c r="D13" s="57">
-        <v>0</v>
-      </c>
-      <c r="E13" s="57">
-        <v>0</v>
-      </c>
-      <c r="F13" s="57">
-        <v>0</v>
-      </c>
-      <c r="G13" s="57">
-        <v>0</v>
-      </c>
-      <c r="H13" s="56">
+      <c r="C13" s="55">
+        <v>0</v>
+      </c>
+      <c r="D13" s="55">
+        <v>0</v>
+      </c>
+      <c r="E13" s="55">
+        <v>0</v>
+      </c>
+      <c r="F13" s="55">
+        <v>0</v>
+      </c>
+      <c r="G13" s="55">
+        <v>0</v>
+      </c>
+      <c r="H13" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="I13" s="56">
+      <c r="I13" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="J13" s="56">
+      <c r="J13" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="K13" s="56">
+      <c r="K13" s="54">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="L13" s="57">
-        <v>0</v>
-      </c>
-      <c r="M13" s="57">
-        <v>0</v>
-      </c>
-      <c r="N13" s="57">
-        <v>0</v>
-      </c>
-      <c r="O13" s="57">
+      <c r="L13" s="55">
+        <v>0</v>
+      </c>
+      <c r="M13" s="55">
+        <v>0</v>
+      </c>
+      <c r="N13" s="55">
+        <v>0</v>
+      </c>
+      <c r="O13" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6560,43 +6560,43 @@
       <c r="B14" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="57">
-        <v>0</v>
-      </c>
-      <c r="D14" s="57">
-        <v>0</v>
-      </c>
-      <c r="E14" s="57">
-        <v>0</v>
-      </c>
-      <c r="F14" s="57">
-        <v>0</v>
-      </c>
-      <c r="G14" s="57">
-        <v>0</v>
-      </c>
-      <c r="H14" s="56">
-        <v>1</v>
-      </c>
-      <c r="I14" s="56">
-        <v>1</v>
-      </c>
-      <c r="J14" s="56">
-        <v>1</v>
-      </c>
-      <c r="K14" s="56">
-        <v>1</v>
-      </c>
-      <c r="L14" s="57">
-        <v>0</v>
-      </c>
-      <c r="M14" s="57">
-        <v>0</v>
-      </c>
-      <c r="N14" s="57">
-        <v>0</v>
-      </c>
-      <c r="O14" s="57">
+      <c r="C14" s="55">
+        <v>0</v>
+      </c>
+      <c r="D14" s="55">
+        <v>0</v>
+      </c>
+      <c r="E14" s="55">
+        <v>0</v>
+      </c>
+      <c r="F14" s="55">
+        <v>0</v>
+      </c>
+      <c r="G14" s="55">
+        <v>0</v>
+      </c>
+      <c r="H14" s="54">
+        <v>1</v>
+      </c>
+      <c r="I14" s="54">
+        <v>1</v>
+      </c>
+      <c r="J14" s="54">
+        <v>1</v>
+      </c>
+      <c r="K14" s="54">
+        <v>1</v>
+      </c>
+      <c r="L14" s="55">
+        <v>0</v>
+      </c>
+      <c r="M14" s="55">
+        <v>0</v>
+      </c>
+      <c r="N14" s="55">
+        <v>0</v>
+      </c>
+      <c r="O14" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6605,47 +6605,47 @@
       <c r="B15" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="C15" s="57">
-        <v>0</v>
-      </c>
-      <c r="D15" s="57">
-        <v>0</v>
-      </c>
-      <c r="E15" s="57">
-        <v>0</v>
-      </c>
-      <c r="F15" s="57">
-        <v>0</v>
-      </c>
-      <c r="G15" s="57">
-        <v>0</v>
-      </c>
-      <c r="H15" s="56">
+      <c r="C15" s="55">
+        <v>0</v>
+      </c>
+      <c r="D15" s="55">
+        <v>0</v>
+      </c>
+      <c r="E15" s="55">
+        <v>0</v>
+      </c>
+      <c r="F15" s="55">
+        <v>0</v>
+      </c>
+      <c r="G15" s="55">
+        <v>0</v>
+      </c>
+      <c r="H15" s="54">
         <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
-      <c r="I15" s="56">
+      <c r="I15" s="54">
         <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
-      <c r="J15" s="56">
+      <c r="J15" s="54">
         <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
-      <c r="K15" s="56">
+      <c r="K15" s="54">
         <f xml:space="preserve"> 1</f>
         <v>1</v>
       </c>
-      <c r="L15" s="57">
-        <v>0</v>
-      </c>
-      <c r="M15" s="57">
-        <v>0</v>
-      </c>
-      <c r="N15" s="57">
-        <v>0</v>
-      </c>
-      <c r="O15" s="57">
+      <c r="L15" s="55">
+        <v>0</v>
+      </c>
+      <c r="M15" s="55">
+        <v>0</v>
+      </c>
+      <c r="N15" s="55">
+        <v>0</v>
+      </c>
+      <c r="O15" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6654,47 +6654,47 @@
       <c r="B16" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="C16" s="57">
-        <v>0</v>
-      </c>
-      <c r="D16" s="57">
-        <v>0</v>
-      </c>
-      <c r="E16" s="57">
-        <v>0</v>
-      </c>
-      <c r="F16" s="57">
-        <v>0</v>
-      </c>
-      <c r="G16" s="57">
-        <v>0</v>
-      </c>
-      <c r="H16" s="56">
+      <c r="C16" s="55">
+        <v>0</v>
+      </c>
+      <c r="D16" s="55">
+        <v>0</v>
+      </c>
+      <c r="E16" s="55">
+        <v>0</v>
+      </c>
+      <c r="F16" s="55">
+        <v>0</v>
+      </c>
+      <c r="G16" s="55">
+        <v>0</v>
+      </c>
+      <c r="H16" s="54">
         <f>frac_PW_health_facility</f>
         <v>0.5</v>
       </c>
-      <c r="I16" s="56">
+      <c r="I16" s="54">
         <f>frac_PW_health_facility</f>
         <v>0.5</v>
       </c>
-      <c r="J16" s="56">
+      <c r="J16" s="54">
         <f>frac_PW_health_facility</f>
         <v>0.5</v>
       </c>
-      <c r="K16" s="56">
+      <c r="K16" s="54">
         <f>frac_PW_health_facility</f>
         <v>0.5</v>
       </c>
-      <c r="L16" s="57">
-        <v>0</v>
-      </c>
-      <c r="M16" s="57">
-        <v>0</v>
-      </c>
-      <c r="N16" s="57">
-        <v>0</v>
-      </c>
-      <c r="O16" s="57">
+      <c r="L16" s="55">
+        <v>0</v>
+      </c>
+      <c r="M16" s="55">
+        <v>0</v>
+      </c>
+      <c r="N16" s="55">
+        <v>0</v>
+      </c>
+      <c r="O16" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6702,47 +6702,47 @@
       <c r="B17" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="57">
-        <v>0</v>
-      </c>
-      <c r="D17" s="57">
-        <v>0</v>
-      </c>
-      <c r="E17" s="57">
-        <v>0</v>
-      </c>
-      <c r="F17" s="57">
-        <v>0</v>
-      </c>
-      <c r="G17" s="57">
-        <v>0</v>
-      </c>
-      <c r="H17" s="56">
+      <c r="C17" s="55">
+        <v>0</v>
+      </c>
+      <c r="D17" s="55">
+        <v>0</v>
+      </c>
+      <c r="E17" s="55">
+        <v>0</v>
+      </c>
+      <c r="F17" s="55">
+        <v>0</v>
+      </c>
+      <c r="G17" s="55">
+        <v>0</v>
+      </c>
+      <c r="H17" s="54">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="I17" s="56">
+      <c r="I17" s="54">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="J17" s="56">
+      <c r="J17" s="54">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="K17" s="56">
+      <c r="K17" s="54">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="L17" s="57">
-        <v>0</v>
-      </c>
-      <c r="M17" s="57">
-        <v>0</v>
-      </c>
-      <c r="N17" s="57">
-        <v>0</v>
-      </c>
-      <c r="O17" s="57">
+      <c r="L17" s="55">
+        <v>0</v>
+      </c>
+      <c r="M17" s="55">
+        <v>0</v>
+      </c>
+      <c r="N17" s="55">
+        <v>0</v>
+      </c>
+      <c r="O17" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6750,43 +6750,43 @@
       <c r="B18" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="57">
-        <v>0</v>
-      </c>
-      <c r="D18" s="57">
-        <v>0</v>
-      </c>
-      <c r="E18" s="57">
-        <v>0</v>
-      </c>
-      <c r="F18" s="57">
-        <v>0</v>
-      </c>
-      <c r="G18" s="57">
-        <v>0</v>
-      </c>
-      <c r="H18" s="56">
-        <v>1</v>
-      </c>
-      <c r="I18" s="56">
-        <v>1</v>
-      </c>
-      <c r="J18" s="56">
-        <v>1</v>
-      </c>
-      <c r="K18" s="56">
-        <v>1</v>
-      </c>
-      <c r="L18" s="57">
-        <v>0</v>
-      </c>
-      <c r="M18" s="57">
-        <v>0</v>
-      </c>
-      <c r="N18" s="57">
-        <v>0</v>
-      </c>
-      <c r="O18" s="57">
+      <c r="C18" s="55">
+        <v>0</v>
+      </c>
+      <c r="D18" s="55">
+        <v>0</v>
+      </c>
+      <c r="E18" s="55">
+        <v>0</v>
+      </c>
+      <c r="F18" s="55">
+        <v>0</v>
+      </c>
+      <c r="G18" s="55">
+        <v>0</v>
+      </c>
+      <c r="H18" s="54">
+        <v>1</v>
+      </c>
+      <c r="I18" s="54">
+        <v>1</v>
+      </c>
+      <c r="J18" s="54">
+        <v>1</v>
+      </c>
+      <c r="K18" s="54">
+        <v>1</v>
+      </c>
+      <c r="L18" s="55">
+        <v>0</v>
+      </c>
+      <c r="M18" s="55">
+        <v>0</v>
+      </c>
+      <c r="N18" s="55">
+        <v>0</v>
+      </c>
+      <c r="O18" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6794,43 +6794,43 @@
       <c r="B19" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="57">
-        <v>0</v>
-      </c>
-      <c r="D19" s="57">
-        <v>0</v>
-      </c>
-      <c r="E19" s="57">
-        <v>0</v>
-      </c>
-      <c r="F19" s="57">
-        <v>0</v>
-      </c>
-      <c r="G19" s="57">
-        <v>0</v>
-      </c>
-      <c r="H19" s="56">
-        <v>1</v>
-      </c>
-      <c r="I19" s="56">
-        <v>1</v>
-      </c>
-      <c r="J19" s="56">
-        <v>1</v>
-      </c>
-      <c r="K19" s="56">
-        <v>1</v>
-      </c>
-      <c r="L19" s="57">
-        <v>0</v>
-      </c>
-      <c r="M19" s="57">
-        <v>0</v>
-      </c>
-      <c r="N19" s="57">
-        <v>0</v>
-      </c>
-      <c r="O19" s="57">
+      <c r="C19" s="55">
+        <v>0</v>
+      </c>
+      <c r="D19" s="55">
+        <v>0</v>
+      </c>
+      <c r="E19" s="55">
+        <v>0</v>
+      </c>
+      <c r="F19" s="55">
+        <v>0</v>
+      </c>
+      <c r="G19" s="55">
+        <v>0</v>
+      </c>
+      <c r="H19" s="54">
+        <v>1</v>
+      </c>
+      <c r="I19" s="54">
+        <v>1</v>
+      </c>
+      <c r="J19" s="54">
+        <v>1</v>
+      </c>
+      <c r="K19" s="54">
+        <v>1</v>
+      </c>
+      <c r="L19" s="55">
+        <v>0</v>
+      </c>
+      <c r="M19" s="55">
+        <v>0</v>
+      </c>
+      <c r="N19" s="55">
+        <v>0</v>
+      </c>
+      <c r="O19" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6838,47 +6838,47 @@
       <c r="B20" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="57">
-        <v>0</v>
-      </c>
-      <c r="D20" s="57">
-        <v>0</v>
-      </c>
-      <c r="E20" s="57">
-        <v>0</v>
-      </c>
-      <c r="F20" s="57">
-        <v>0</v>
-      </c>
-      <c r="G20" s="57">
-        <v>0</v>
-      </c>
-      <c r="H20" s="56">
+      <c r="C20" s="55">
+        <v>0</v>
+      </c>
+      <c r="D20" s="55">
+        <v>0</v>
+      </c>
+      <c r="E20" s="55">
+        <v>0</v>
+      </c>
+      <c r="F20" s="55">
+        <v>0</v>
+      </c>
+      <c r="G20" s="55">
+        <v>0</v>
+      </c>
+      <c r="H20" s="54">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="I20" s="56">
+      <c r="I20" s="54">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="J20" s="56">
+      <c r="J20" s="54">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="K20" s="56">
+      <c r="K20" s="54">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="L20" s="57">
-        <v>0</v>
-      </c>
-      <c r="M20" s="57">
-        <v>0</v>
-      </c>
-      <c r="N20" s="57">
-        <v>0</v>
-      </c>
-      <c r="O20" s="57">
+      <c r="L20" s="55">
+        <v>0</v>
+      </c>
+      <c r="M20" s="55">
+        <v>0</v>
+      </c>
+      <c r="N20" s="55">
+        <v>0</v>
+      </c>
+      <c r="O20" s="55">
         <v>0</v>
       </c>
     </row>
@@ -6886,282 +6886,282 @@
       <c r="B21" s="52"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="101" t="s">
+      <c r="A22" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="103" t="s">
+      <c r="B22" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="57">
-        <v>0</v>
-      </c>
-      <c r="D22" s="57">
-        <v>0</v>
-      </c>
-      <c r="E22" s="57">
-        <v>0</v>
-      </c>
-      <c r="F22" s="57">
-        <v>0</v>
-      </c>
-      <c r="G22" s="57">
-        <v>0</v>
-      </c>
-      <c r="H22" s="57">
-        <v>0</v>
-      </c>
-      <c r="I22" s="57">
-        <v>0</v>
-      </c>
-      <c r="J22" s="57">
-        <v>0</v>
-      </c>
-      <c r="K22" s="57">
-        <v>0</v>
-      </c>
-      <c r="L22" s="58">
-        <v>1</v>
-      </c>
-      <c r="M22" s="58">
-        <v>1</v>
-      </c>
-      <c r="N22" s="58">
-        <v>1</v>
-      </c>
-      <c r="O22" s="58">
+      <c r="C22" s="55">
+        <v>0</v>
+      </c>
+      <c r="D22" s="55">
+        <v>0</v>
+      </c>
+      <c r="E22" s="55">
+        <v>0</v>
+      </c>
+      <c r="F22" s="55">
+        <v>0</v>
+      </c>
+      <c r="G22" s="55">
+        <v>0</v>
+      </c>
+      <c r="H22" s="55">
+        <v>0</v>
+      </c>
+      <c r="I22" s="55">
+        <v>0</v>
+      </c>
+      <c r="J22" s="55">
+        <v>0</v>
+      </c>
+      <c r="K22" s="55">
+        <v>0</v>
+      </c>
+      <c r="L22" s="56">
+        <v>1</v>
+      </c>
+      <c r="M22" s="56">
+        <v>1</v>
+      </c>
+      <c r="N22" s="56">
+        <v>1</v>
+      </c>
+      <c r="O22" s="56">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="103" t="s">
+      <c r="B23" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="57">
-        <v>0</v>
-      </c>
-      <c r="D23" s="57">
-        <v>0</v>
-      </c>
-      <c r="E23" s="57">
-        <v>0</v>
-      </c>
-      <c r="F23" s="57">
-        <v>0</v>
-      </c>
-      <c r="G23" s="57">
-        <v>0</v>
-      </c>
-      <c r="H23" s="57">
-        <v>0</v>
-      </c>
-      <c r="I23" s="57">
-        <v>0</v>
-      </c>
-      <c r="J23" s="57">
-        <v>0</v>
-      </c>
-      <c r="K23" s="57">
-        <v>0</v>
-      </c>
-      <c r="L23" s="56">
-        <v>1</v>
-      </c>
-      <c r="M23" s="56">
-        <v>1</v>
-      </c>
-      <c r="N23" s="56">
-        <v>1</v>
-      </c>
-      <c r="O23" s="56">
+      <c r="C23" s="55">
+        <v>0</v>
+      </c>
+      <c r="D23" s="55">
+        <v>0</v>
+      </c>
+      <c r="E23" s="55">
+        <v>0</v>
+      </c>
+      <c r="F23" s="55">
+        <v>0</v>
+      </c>
+      <c r="G23" s="55">
+        <v>0</v>
+      </c>
+      <c r="H23" s="55">
+        <v>0</v>
+      </c>
+      <c r="I23" s="55">
+        <v>0</v>
+      </c>
+      <c r="J23" s="55">
+        <v>0</v>
+      </c>
+      <c r="K23" s="55">
+        <v>0</v>
+      </c>
+      <c r="L23" s="54">
+        <v>1</v>
+      </c>
+      <c r="M23" s="54">
+        <v>1</v>
+      </c>
+      <c r="N23" s="54">
+        <v>1</v>
+      </c>
+      <c r="O23" s="54">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="101" t="s">
         <v>218</v>
       </c>
-      <c r="C24" s="57">
-        <v>0</v>
-      </c>
-      <c r="D24" s="57">
-        <v>0</v>
-      </c>
-      <c r="E24" s="57">
-        <v>0</v>
-      </c>
-      <c r="F24" s="57">
-        <v>0</v>
-      </c>
-      <c r="G24" s="57">
-        <v>0</v>
-      </c>
-      <c r="H24" s="57">
-        <v>0</v>
-      </c>
-      <c r="I24" s="57">
-        <v>0</v>
-      </c>
-      <c r="J24" s="57">
-        <v>0</v>
-      </c>
-      <c r="K24" s="57">
-        <v>0</v>
-      </c>
-      <c r="L24" s="56">
+      <c r="C24" s="55">
+        <v>0</v>
+      </c>
+      <c r="D24" s="55">
+        <v>0</v>
+      </c>
+      <c r="E24" s="55">
+        <v>0</v>
+      </c>
+      <c r="F24" s="55">
+        <v>0</v>
+      </c>
+      <c r="G24" s="55">
+        <v>0</v>
+      </c>
+      <c r="H24" s="55">
+        <v>0</v>
+      </c>
+      <c r="I24" s="55">
+        <v>0</v>
+      </c>
+      <c r="J24" s="55">
+        <v>0</v>
+      </c>
+      <c r="K24" s="55">
+        <v>0</v>
+      </c>
+      <c r="L24" s="54">
         <f>(1-food_insecure)*(0.49)*(1-school_attendance) + food_insecure*(0.7)*(1-school_attendance)</f>
         <v>0.36650879999999997</v>
       </c>
-      <c r="M24" s="56">
+      <c r="M24" s="54">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
         <v>0.56559999999999999</v>
       </c>
-      <c r="N24" s="56">
+      <c r="N24" s="54">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
         <v>0.56559999999999999</v>
       </c>
-      <c r="O24" s="56">
+      <c r="O24" s="54">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
         <v>0.56559999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="103" t="s">
+      <c r="B25" s="101" t="s">
         <v>219</v>
       </c>
-      <c r="C25" s="57">
-        <v>0</v>
-      </c>
-      <c r="D25" s="57">
-        <v>0</v>
-      </c>
-      <c r="E25" s="57">
-        <v>0</v>
-      </c>
-      <c r="F25" s="57">
-        <v>0</v>
-      </c>
-      <c r="G25" s="57">
-        <v>0</v>
-      </c>
-      <c r="H25" s="57">
-        <v>0</v>
-      </c>
-      <c r="I25" s="57">
-        <v>0</v>
-      </c>
-      <c r="J25" s="57">
-        <v>0</v>
-      </c>
-      <c r="K25" s="57">
-        <v>0</v>
-      </c>
-      <c r="L25" s="56">
+      <c r="C25" s="55">
+        <v>0</v>
+      </c>
+      <c r="D25" s="55">
+        <v>0</v>
+      </c>
+      <c r="E25" s="55">
+        <v>0</v>
+      </c>
+      <c r="F25" s="55">
+        <v>0</v>
+      </c>
+      <c r="G25" s="55">
+        <v>0</v>
+      </c>
+      <c r="H25" s="55">
+        <v>0</v>
+      </c>
+      <c r="I25" s="55">
+        <v>0</v>
+      </c>
+      <c r="J25" s="55">
+        <v>0</v>
+      </c>
+      <c r="K25" s="55">
+        <v>0</v>
+      </c>
+      <c r="L25" s="54">
         <f>(1-food_insecure)*(0.21)*(1-school_attendance) + food_insecure*(0.3)*(1-school_attendance)</f>
         <v>0.1570752</v>
       </c>
-      <c r="M25" s="56">
+      <c r="M25" s="54">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
         <v>0.2424</v>
       </c>
-      <c r="N25" s="56">
+      <c r="N25" s="54">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
         <v>0.2424</v>
       </c>
-      <c r="O25" s="56">
+      <c r="O25" s="54">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
         <v>0.2424</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="101" t="s">
         <v>220</v>
       </c>
-      <c r="C26" s="57">
-        <v>0</v>
-      </c>
-      <c r="D26" s="57">
-        <v>0</v>
-      </c>
-      <c r="E26" s="57">
-        <v>0</v>
-      </c>
-      <c r="F26" s="57">
-        <v>0</v>
-      </c>
-      <c r="G26" s="57">
-        <v>0</v>
-      </c>
-      <c r="H26" s="57">
-        <v>0</v>
-      </c>
-      <c r="I26" s="57">
-        <v>0</v>
-      </c>
-      <c r="J26" s="57">
-        <v>0</v>
-      </c>
-      <c r="K26" s="57">
-        <v>0</v>
-      </c>
-      <c r="L26" s="56">
+      <c r="C26" s="55">
+        <v>0</v>
+      </c>
+      <c r="D26" s="55">
+        <v>0</v>
+      </c>
+      <c r="E26" s="55">
+        <v>0</v>
+      </c>
+      <c r="F26" s="55">
+        <v>0</v>
+      </c>
+      <c r="G26" s="55">
+        <v>0</v>
+      </c>
+      <c r="H26" s="55">
+        <v>0</v>
+      </c>
+      <c r="I26" s="55">
+        <v>0</v>
+      </c>
+      <c r="J26" s="55">
+        <v>0</v>
+      </c>
+      <c r="K26" s="55">
+        <v>0</v>
+      </c>
+      <c r="L26" s="54">
         <f>(1-food_insecure)*(0.3)*(1-school_attendance)</f>
         <v>0.12441600000000001</v>
       </c>
-      <c r="M26" s="56">
+      <c r="M26" s="54">
         <f>(1-food_insecure)*(0.3)</f>
         <v>0.192</v>
       </c>
-      <c r="N26" s="56">
+      <c r="N26" s="54">
         <f>(1-food_insecure)*(0.3)</f>
         <v>0.192</v>
       </c>
-      <c r="O26" s="56">
+      <c r="O26" s="54">
         <f>(1-food_insecure)*(0.3)</f>
         <v>0.192</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="103" t="s">
+      <c r="B27" s="101" t="s">
         <v>221</v>
       </c>
-      <c r="C27" s="57">
-        <v>0</v>
-      </c>
-      <c r="D27" s="57">
-        <v>0</v>
-      </c>
-      <c r="E27" s="57">
-        <v>0</v>
-      </c>
-      <c r="F27" s="57">
-        <v>0</v>
-      </c>
-      <c r="G27" s="57">
-        <v>0</v>
-      </c>
-      <c r="H27" s="57">
-        <v>0</v>
-      </c>
-      <c r="I27" s="57">
-        <v>0</v>
-      </c>
-      <c r="J27" s="57">
-        <v>0</v>
-      </c>
-      <c r="K27" s="57">
-        <v>0</v>
-      </c>
-      <c r="L27" s="56">
+      <c r="C27" s="55">
+        <v>0</v>
+      </c>
+      <c r="D27" s="55">
+        <v>0</v>
+      </c>
+      <c r="E27" s="55">
+        <v>0</v>
+      </c>
+      <c r="F27" s="55">
+        <v>0</v>
+      </c>
+      <c r="G27" s="55">
+        <v>0</v>
+      </c>
+      <c r="H27" s="55">
+        <v>0</v>
+      </c>
+      <c r="I27" s="55">
+        <v>0</v>
+      </c>
+      <c r="J27" s="55">
+        <v>0</v>
+      </c>
+      <c r="K27" s="55">
+        <v>0</v>
+      </c>
+      <c r="L27" s="54">
         <f>(1-food_insecure)*1*school_attendance + food_insecure*1*school_attendance</f>
         <v>0.35199999999999998</v>
       </c>
-      <c r="M27" s="56">
-        <v>0</v>
-      </c>
-      <c r="N27" s="56">
-        <v>0</v>
-      </c>
-      <c r="O27" s="56">
+      <c r="M27" s="54">
+        <v>0</v>
+      </c>
+      <c r="N27" s="54">
+        <v>0</v>
+      </c>
+      <c r="O27" s="54">
         <v>0</v>
       </c>
     </row>
@@ -7182,53 +7182,53 @@
       <c r="B29" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="56">
-        <v>0</v>
-      </c>
-      <c r="D29" s="56">
-        <v>0</v>
-      </c>
-      <c r="E29" s="56">
+      <c r="C29" s="54">
+        <v>0</v>
+      </c>
+      <c r="D29" s="54">
+        <v>0</v>
+      </c>
+      <c r="E29" s="54">
         <f t="shared" ref="E29:O29" si="0">frac_maize</f>
         <v>0.05</v>
       </c>
-      <c r="F29" s="56">
+      <c r="F29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="G29" s="56">
+      <c r="G29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="H29" s="56">
+      <c r="H29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="I29" s="56">
+      <c r="I29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="J29" s="56">
+      <c r="J29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="K29" s="56">
+      <c r="K29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="L29" s="56">
+      <c r="L29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="M29" s="56">
+      <c r="M29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="N29" s="56">
+      <c r="N29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="O29" s="56">
+      <c r="O29" s="54">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
@@ -7237,53 +7237,53 @@
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="56">
-        <v>0</v>
-      </c>
-      <c r="D30" s="56">
-        <v>0</v>
-      </c>
-      <c r="E30" s="56">
+      <c r="C30" s="54">
+        <v>0</v>
+      </c>
+      <c r="D30" s="54">
+        <v>0</v>
+      </c>
+      <c r="E30" s="54">
         <f t="shared" ref="E30:O30" si="1">frac_rice</f>
         <v>0.8</v>
       </c>
-      <c r="F30" s="56">
+      <c r="F30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="G30" s="56">
+      <c r="G30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H30" s="56">
+      <c r="H30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="I30" s="56">
+      <c r="I30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="J30" s="56">
+      <c r="J30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="K30" s="56">
+      <c r="K30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="L30" s="56">
+      <c r="L30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="M30" s="56">
+      <c r="M30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="N30" s="56">
+      <c r="N30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="O30" s="56">
+      <c r="O30" s="54">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
@@ -7292,53 +7292,53 @@
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="56">
-        <v>0</v>
-      </c>
-      <c r="D31" s="56">
-        <v>0</v>
-      </c>
-      <c r="E31" s="56">
+      <c r="C31" s="54">
+        <v>0</v>
+      </c>
+      <c r="D31" s="54">
+        <v>0</v>
+      </c>
+      <c r="E31" s="54">
         <f t="shared" ref="E31:O31" si="2">frac_wheat</f>
         <v>0.12</v>
       </c>
-      <c r="F31" s="56">
+      <c r="F31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="G31" s="56">
+      <c r="G31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="H31" s="56">
+      <c r="H31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="I31" s="56">
+      <c r="I31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="J31" s="56">
+      <c r="J31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="K31" s="56">
+      <c r="K31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="L31" s="56">
+      <c r="L31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="M31" s="56">
+      <c r="M31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="N31" s="56">
+      <c r="N31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="O31" s="56">
+      <c r="O31" s="54">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
@@ -7347,43 +7347,43 @@
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="56">
-        <v>0</v>
-      </c>
-      <c r="D32" s="56">
-        <v>0</v>
-      </c>
-      <c r="E32" s="56">
-        <v>1</v>
-      </c>
-      <c r="F32" s="56">
-        <v>1</v>
-      </c>
-      <c r="G32" s="56">
-        <v>1</v>
-      </c>
-      <c r="H32" s="56">
-        <v>1</v>
-      </c>
-      <c r="I32" s="56">
-        <v>1</v>
-      </c>
-      <c r="J32" s="56">
-        <v>1</v>
-      </c>
-      <c r="K32" s="56">
-        <v>1</v>
-      </c>
-      <c r="L32" s="56">
-        <v>1</v>
-      </c>
-      <c r="M32" s="56">
-        <v>1</v>
-      </c>
-      <c r="N32" s="56">
-        <v>1</v>
-      </c>
-      <c r="O32" s="56">
+      <c r="C32" s="54">
+        <v>0</v>
+      </c>
+      <c r="D32" s="54">
+        <v>0</v>
+      </c>
+      <c r="E32" s="54">
+        <v>1</v>
+      </c>
+      <c r="F32" s="54">
+        <v>1</v>
+      </c>
+      <c r="G32" s="54">
+        <v>1</v>
+      </c>
+      <c r="H32" s="54">
+        <v>1</v>
+      </c>
+      <c r="I32" s="54">
+        <v>1</v>
+      </c>
+      <c r="J32" s="54">
+        <v>1</v>
+      </c>
+      <c r="K32" s="54">
+        <v>1</v>
+      </c>
+      <c r="L32" s="54">
+        <v>1</v>
+      </c>
+      <c r="M32" s="54">
+        <v>1</v>
+      </c>
+      <c r="N32" s="54">
+        <v>1</v>
+      </c>
+      <c r="O32" s="54">
         <v>1</v>
       </c>
     </row>
@@ -7391,55 +7391,55 @@
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="56">
+      <c r="C33" s="54">
         <f t="shared" ref="C33:O33" si="3">frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="D33" s="56">
+      <c r="D33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="E33" s="56">
+      <c r="E33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="F33" s="56">
+      <c r="F33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="G33" s="56">
+      <c r="G33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="H33" s="56">
+      <c r="H33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="I33" s="56">
+      <c r="I33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="J33" s="56">
+      <c r="J33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="K33" s="56">
+      <c r="K33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="L33" s="56">
+      <c r="L33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="M33" s="56">
+      <c r="M33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="N33" s="56">
+      <c r="N33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="O33" s="56">
+      <c r="O33" s="54">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
@@ -7448,43 +7448,43 @@
       <c r="B34" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="56">
-        <v>1</v>
-      </c>
-      <c r="D34" s="56">
-        <v>1</v>
-      </c>
-      <c r="E34" s="56">
-        <v>1</v>
-      </c>
-      <c r="F34" s="56">
-        <v>1</v>
-      </c>
-      <c r="G34" s="56">
-        <v>1</v>
-      </c>
-      <c r="H34" s="56">
-        <v>1</v>
-      </c>
-      <c r="I34" s="56">
-        <v>1</v>
-      </c>
-      <c r="J34" s="56">
-        <v>1</v>
-      </c>
-      <c r="K34" s="56">
-        <v>1</v>
-      </c>
-      <c r="L34" s="56">
-        <v>1</v>
-      </c>
-      <c r="M34" s="56">
-        <v>1</v>
-      </c>
-      <c r="N34" s="56">
-        <v>1</v>
-      </c>
-      <c r="O34" s="56">
+      <c r="C34" s="54">
+        <v>1</v>
+      </c>
+      <c r="D34" s="54">
+        <v>1</v>
+      </c>
+      <c r="E34" s="54">
+        <v>1</v>
+      </c>
+      <c r="F34" s="54">
+        <v>1</v>
+      </c>
+      <c r="G34" s="54">
+        <v>1</v>
+      </c>
+      <c r="H34" s="54">
+        <v>1</v>
+      </c>
+      <c r="I34" s="54">
+        <v>1</v>
+      </c>
+      <c r="J34" s="54">
+        <v>1</v>
+      </c>
+      <c r="K34" s="54">
+        <v>1</v>
+      </c>
+      <c r="L34" s="54">
+        <v>1</v>
+      </c>
+      <c r="M34" s="54">
+        <v>1</v>
+      </c>
+      <c r="N34" s="54">
+        <v>1</v>
+      </c>
+      <c r="O34" s="54">
         <v>1</v>
       </c>
     </row>
@@ -7493,43 +7493,43 @@
       <c r="B35" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="56">
-        <v>1</v>
-      </c>
-      <c r="D35" s="56">
-        <v>1</v>
-      </c>
-      <c r="E35" s="56">
-        <v>1</v>
-      </c>
-      <c r="F35" s="56">
-        <v>1</v>
-      </c>
-      <c r="G35" s="56">
-        <v>1</v>
-      </c>
-      <c r="H35" s="56">
-        <v>1</v>
-      </c>
-      <c r="I35" s="56">
-        <v>1</v>
-      </c>
-      <c r="J35" s="56">
-        <v>1</v>
-      </c>
-      <c r="K35" s="56">
-        <v>1</v>
-      </c>
-      <c r="L35" s="56">
-        <v>1</v>
-      </c>
-      <c r="M35" s="56">
-        <v>1</v>
-      </c>
-      <c r="N35" s="56">
-        <v>1</v>
-      </c>
-      <c r="O35" s="56">
+      <c r="C35" s="54">
+        <v>1</v>
+      </c>
+      <c r="D35" s="54">
+        <v>1</v>
+      </c>
+      <c r="E35" s="54">
+        <v>1</v>
+      </c>
+      <c r="F35" s="54">
+        <v>1</v>
+      </c>
+      <c r="G35" s="54">
+        <v>1</v>
+      </c>
+      <c r="H35" s="54">
+        <v>1</v>
+      </c>
+      <c r="I35" s="54">
+        <v>1</v>
+      </c>
+      <c r="J35" s="54">
+        <v>1</v>
+      </c>
+      <c r="K35" s="54">
+        <v>1</v>
+      </c>
+      <c r="L35" s="54">
+        <v>1</v>
+      </c>
+      <c r="M35" s="54">
+        <v>1</v>
+      </c>
+      <c r="N35" s="54">
+        <v>1</v>
+      </c>
+      <c r="O35" s="54">
         <v>1</v>
       </c>
     </row>
@@ -7537,43 +7537,43 @@
       <c r="B36" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="56">
-        <v>1</v>
-      </c>
-      <c r="D36" s="56">
-        <v>1</v>
-      </c>
-      <c r="E36" s="56">
-        <v>1</v>
-      </c>
-      <c r="F36" s="56">
-        <v>1</v>
-      </c>
-      <c r="G36" s="56">
-        <v>1</v>
-      </c>
-      <c r="H36" s="56">
-        <v>1</v>
-      </c>
-      <c r="I36" s="56">
-        <v>1</v>
-      </c>
-      <c r="J36" s="56">
-        <v>1</v>
-      </c>
-      <c r="K36" s="56">
-        <v>1</v>
-      </c>
-      <c r="L36" s="56">
-        <v>1</v>
-      </c>
-      <c r="M36" s="56">
-        <v>1</v>
-      </c>
-      <c r="N36" s="56">
-        <v>1</v>
-      </c>
-      <c r="O36" s="56">
+      <c r="C36" s="54">
+        <v>1</v>
+      </c>
+      <c r="D36" s="54">
+        <v>1</v>
+      </c>
+      <c r="E36" s="54">
+        <v>1</v>
+      </c>
+      <c r="F36" s="54">
+        <v>1</v>
+      </c>
+      <c r="G36" s="54">
+        <v>1</v>
+      </c>
+      <c r="H36" s="54">
+        <v>1</v>
+      </c>
+      <c r="I36" s="54">
+        <v>1</v>
+      </c>
+      <c r="J36" s="54">
+        <v>1</v>
+      </c>
+      <c r="K36" s="54">
+        <v>1</v>
+      </c>
+      <c r="L36" s="54">
+        <v>1</v>
+      </c>
+      <c r="M36" s="54">
+        <v>1</v>
+      </c>
+      <c r="N36" s="54">
+        <v>1</v>
+      </c>
+      <c r="O36" s="54">
         <v>1</v>
       </c>
     </row>
@@ -7581,43 +7581,43 @@
       <c r="B37" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="56">
-        <v>1</v>
-      </c>
-      <c r="D37" s="56">
-        <v>1</v>
-      </c>
-      <c r="E37" s="56">
-        <v>1</v>
-      </c>
-      <c r="F37" s="56">
-        <v>1</v>
-      </c>
-      <c r="G37" s="56">
-        <v>1</v>
-      </c>
-      <c r="H37" s="56">
-        <v>1</v>
-      </c>
-      <c r="I37" s="56">
-        <v>1</v>
-      </c>
-      <c r="J37" s="56">
-        <v>1</v>
-      </c>
-      <c r="K37" s="56">
-        <v>1</v>
-      </c>
-      <c r="L37" s="56">
-        <v>1</v>
-      </c>
-      <c r="M37" s="56">
-        <v>1</v>
-      </c>
-      <c r="N37" s="56">
-        <v>1</v>
-      </c>
-      <c r="O37" s="56">
+      <c r="C37" s="54">
+        <v>1</v>
+      </c>
+      <c r="D37" s="54">
+        <v>1</v>
+      </c>
+      <c r="E37" s="54">
+        <v>1</v>
+      </c>
+      <c r="F37" s="54">
+        <v>1</v>
+      </c>
+      <c r="G37" s="54">
+        <v>1</v>
+      </c>
+      <c r="H37" s="54">
+        <v>1</v>
+      </c>
+      <c r="I37" s="54">
+        <v>1</v>
+      </c>
+      <c r="J37" s="54">
+        <v>1</v>
+      </c>
+      <c r="K37" s="54">
+        <v>1</v>
+      </c>
+      <c r="L37" s="54">
+        <v>1</v>
+      </c>
+      <c r="M37" s="54">
+        <v>1</v>
+      </c>
+      <c r="N37" s="54">
+        <v>1</v>
+      </c>
+      <c r="O37" s="54">
         <v>1</v>
       </c>
     </row>
@@ -7625,43 +7625,43 @@
       <c r="B38" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="56">
-        <v>1</v>
-      </c>
-      <c r="D38" s="56">
-        <v>1</v>
-      </c>
-      <c r="E38" s="56">
-        <v>1</v>
-      </c>
-      <c r="F38" s="56">
-        <v>1</v>
-      </c>
-      <c r="G38" s="56">
-        <v>1</v>
-      </c>
-      <c r="H38" s="56">
-        <v>1</v>
-      </c>
-      <c r="I38" s="56">
-        <v>1</v>
-      </c>
-      <c r="J38" s="56">
-        <v>1</v>
-      </c>
-      <c r="K38" s="56">
-        <v>1</v>
-      </c>
-      <c r="L38" s="56">
-        <v>1</v>
-      </c>
-      <c r="M38" s="56">
-        <v>1</v>
-      </c>
-      <c r="N38" s="56">
-        <v>1</v>
-      </c>
-      <c r="O38" s="56">
+      <c r="C38" s="54">
+        <v>1</v>
+      </c>
+      <c r="D38" s="54">
+        <v>1</v>
+      </c>
+      <c r="E38" s="54">
+        <v>1</v>
+      </c>
+      <c r="F38" s="54">
+        <v>1</v>
+      </c>
+      <c r="G38" s="54">
+        <v>1</v>
+      </c>
+      <c r="H38" s="54">
+        <v>1</v>
+      </c>
+      <c r="I38" s="54">
+        <v>1</v>
+      </c>
+      <c r="J38" s="54">
+        <v>1</v>
+      </c>
+      <c r="K38" s="54">
+        <v>1</v>
+      </c>
+      <c r="L38" s="54">
+        <v>1</v>
+      </c>
+      <c r="M38" s="54">
+        <v>1</v>
+      </c>
+      <c r="N38" s="54">
+        <v>1</v>
+      </c>
+      <c r="O38" s="54">
         <v>1</v>
       </c>
     </row>
@@ -7691,194 +7691,194 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="60" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="60" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="60"/>
-    <col min="5" max="5" width="17.5" style="60" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="60"/>
+    <col min="1" max="1" width="33.6640625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="58" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="58"/>
+    <col min="5" max="5" width="17.5" style="58" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="63" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="63">
+      <c r="B2" s="61">
         <v>0.9</v>
       </c>
-      <c r="C2" s="62">
+      <c r="C2" s="60">
         <v>0.09</v>
       </c>
-      <c r="D2" s="60">
+      <c r="D2" s="58">
         <v>0.8</v>
       </c>
-      <c r="E2" s="60">
+      <c r="E2" s="58">
         <f t="shared" ref="E2:E10" si="0">C2*D2</f>
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="63">
-        <v>1</v>
-      </c>
-      <c r="C3" s="62">
+      <c r="B3" s="61">
+        <v>1</v>
+      </c>
+      <c r="C3" s="60">
         <v>0.02</v>
       </c>
-      <c r="D3" s="60">
+      <c r="D3" s="58">
         <v>1.9</v>
       </c>
-      <c r="E3" s="60">
+      <c r="E3" s="58">
         <f t="shared" si="0"/>
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="B4" s="63">
-        <v>1</v>
-      </c>
-      <c r="C4" s="62">
+      <c r="B4" s="61">
+        <v>1</v>
+      </c>
+      <c r="C4" s="60">
         <v>0.08</v>
       </c>
-      <c r="D4" s="60">
+      <c r="D4" s="58">
         <v>2</v>
       </c>
-      <c r="E4" s="60">
+      <c r="E4" s="58">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="63">
-        <v>1</v>
-      </c>
-      <c r="C5" s="62">
+      <c r="B5" s="61">
+        <v>1</v>
+      </c>
+      <c r="C5" s="60">
         <v>0.18</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="58">
         <v>0.7</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="58">
         <f t="shared" si="0"/>
         <v>0.126</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="B6" s="63">
-        <v>1</v>
-      </c>
-      <c r="C6" s="62">
+      <c r="B6" s="61">
+        <v>1</v>
+      </c>
+      <c r="C6" s="60">
         <v>0.02</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="58">
         <v>0.7</v>
       </c>
-      <c r="E6" s="60">
+      <c r="E6" s="58">
         <f t="shared" si="0"/>
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="B7" s="63">
+      <c r="B7" s="61">
         <v>0.93</v>
       </c>
-      <c r="C7" s="62">
+      <c r="C7" s="60">
         <v>0.45</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="58">
         <v>0.9</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="58">
         <f t="shared" si="0"/>
         <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="63">
+      <c r="B8" s="61">
         <v>0.5</v>
       </c>
-      <c r="C8" s="62">
+      <c r="C8" s="60">
         <v>0.03</v>
       </c>
-      <c r="D8" s="60">
-        <v>0</v>
-      </c>
-      <c r="E8" s="60">
+      <c r="D8" s="58">
+        <v>0</v>
+      </c>
+      <c r="E8" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="63">
+      <c r="B9" s="61">
         <v>0.5</v>
       </c>
-      <c r="C9" s="62">
+      <c r="C9" s="60">
         <v>0.11</v>
       </c>
-      <c r="D9" s="60">
-        <v>0</v>
-      </c>
-      <c r="E9" s="60">
+      <c r="D9" s="58">
+        <v>0</v>
+      </c>
+      <c r="E9" s="58">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="63">
+      <c r="B10" s="61">
         <v>0.98</v>
       </c>
-      <c r="C10" s="62">
+      <c r="C10" s="60">
         <v>0.01</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="58">
         <v>0.6</v>
       </c>
-      <c r="E10" s="60">
+      <c r="E10" s="58">
         <f t="shared" si="0"/>
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="C11" s="61"/>
+      <c r="C11" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8540,15 +8540,15 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
     <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="16" customWidth="1"/>
     <col min="12" max="12" width="16.83203125" style="15" customWidth="1"/>
     <col min="13" max="16384" width="14.5" style="15"/>
   </cols>
@@ -8584,7 +8584,7 @@
       <c r="J1" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="104" t="s">
         <v>149</v>
       </c>
       <c r="L1" s="31" t="s">
@@ -8624,7 +8624,7 @@
         <f t="shared" ref="J2:J15" si="1">(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
         <v>3650590.4685349194</v>
       </c>
-      <c r="K2" s="55">
+      <c r="K2" s="105">
         <f t="shared" ref="K2:K15" si="2">D2/I2</f>
         <v>0.19650809343064388</v>
       </c>
@@ -8666,7 +8666,7 @@
         <f t="shared" si="1"/>
         <v>3622037.632993402</v>
       </c>
-      <c r="K3" s="55">
+      <c r="K3" s="105">
         <f t="shared" si="2"/>
         <v>0.19560012431005733</v>
       </c>
@@ -8708,7 +8708,7 @@
         <f t="shared" si="1"/>
         <v>3591353.7424015561</v>
       </c>
-      <c r="K4" s="55">
+      <c r="K4" s="105">
         <f t="shared" si="2"/>
         <v>0.19473040344679096</v>
       </c>
@@ -8750,7 +8750,7 @@
         <f t="shared" si="1"/>
         <v>3558361.8967828737</v>
       </c>
-      <c r="K5" s="55">
+      <c r="K5" s="105">
         <f t="shared" si="2"/>
         <v>0.19389656387960991</v>
       </c>
@@ -8792,7 +8792,7 @@
         <f t="shared" si="1"/>
         <v>3527004.6069471212</v>
       </c>
-      <c r="K6" s="55">
+      <c r="K6" s="105">
         <f t="shared" si="2"/>
         <v>0.1930964300031866</v>
       </c>
@@ -8834,7 +8834,7 @@
         <f t="shared" si="1"/>
         <v>3493354.6934158299</v>
       </c>
-      <c r="K7" s="55">
+      <c r="K7" s="105">
         <f t="shared" si="2"/>
         <v>0.1833447699409301</v>
       </c>
@@ -8876,7 +8876,7 @@
         <f t="shared" si="1"/>
         <v>3457383.8521927581</v>
       </c>
-      <c r="K8" s="55">
+      <c r="K8" s="105">
         <f t="shared" si="2"/>
         <v>0.17377791134121673</v>
       </c>
@@ -8918,7 +8918,7 @@
         <f t="shared" si="1"/>
         <v>3419187.609265219</v>
       </c>
-      <c r="K9" s="55">
+      <c r="K9" s="105">
         <f t="shared" si="2"/>
         <v>0.16439065031797631</v>
       </c>
@@ -8960,7 +8960,7 @@
         <f t="shared" si="1"/>
         <v>3378798.9859621613</v>
       </c>
-      <c r="K10" s="55">
+      <c r="K10" s="105">
         <f t="shared" si="2"/>
         <v>0.15517797655218554</v>
       </c>
@@ -9002,7 +9002,7 @@
         <f t="shared" si="1"/>
         <v>3344756.3544830228</v>
       </c>
-      <c r="K11" s="55">
+      <c r="K11" s="105">
         <f t="shared" si="2"/>
         <v>0.1461350643747365</v>
       </c>
@@ -9044,7 +9044,7 @@
         <f t="shared" si="1"/>
         <v>3308667.5799422786</v>
       </c>
-      <c r="K12" s="55">
+      <c r="K12" s="105">
         <f t="shared" si="2"/>
         <v>0.14438357872262508</v>
       </c>
@@ -9086,7 +9086,7 @@
         <f t="shared" si="1"/>
         <v>3270569.2216684073</v>
       </c>
-      <c r="K13" s="55">
+      <c r="K13" s="105">
         <f t="shared" si="2"/>
         <v>0.14265533716616713</v>
       </c>
@@ -9128,7 +9128,7 @@
         <f t="shared" si="1"/>
         <v>3230515.5289875376</v>
       </c>
-      <c r="K14" s="55">
+      <c r="K14" s="105">
         <f t="shared" si="2"/>
         <v>0.14094988004429135</v>
       </c>
@@ -9170,7 +9170,7 @@
         <f t="shared" si="1"/>
         <v>3188527.7298968509</v>
       </c>
-      <c r="K15" s="55">
+      <c r="K15" s="105">
         <f t="shared" si="2"/>
         <v>0.139266759736527</v>
       </c>
@@ -9654,7 +9654,7 @@
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="67" t="s">
         <v>189</v>
       </c>
       <c r="C2" s="39">
@@ -9674,7 +9674,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="67" t="s">
         <v>190</v>
       </c>
       <c r="C3" s="39">
@@ -9694,7 +9694,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="67" t="s">
         <v>191</v>
       </c>
       <c r="C4" s="39">
@@ -9714,7 +9714,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="67" t="s">
         <v>192</v>
       </c>
       <c r="C5" s="49">
@@ -9971,7 +9971,7 @@
       <c r="A1" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="65" t="s">
         <v>187</v>
       </c>
       <c r="C1" s="43" t="s">
@@ -10129,251 +10129,251 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17" style="60" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="60" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="60" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="60"/>
+    <col min="1" max="1" width="17" style="58" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="58" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="79" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="79" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="79" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="E2" s="99" t="str">
+      <c r="E2" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="74"/>
-      <c r="B3" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="99" t="str">
+      <c r="A3" s="72"/>
+      <c r="B3" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="74"/>
-      <c r="B4" s="73" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="99" t="str">
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="74"/>
-      <c r="B5" s="73" t="s">
+      <c r="A5" s="72"/>
+      <c r="B5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="99" t="str">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="74"/>
-      <c r="B6" s="73" t="s">
+      <c r="A6" s="72"/>
+      <c r="B6" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="99" t="str">
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="74"/>
-      <c r="B7" s="73" t="s">
+      <c r="A7" s="72"/>
+      <c r="B7" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="76"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="74"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="78" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="79" t="s">
+      <c r="B9" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="100" t="str">
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="98" t="str">
         <f>IF(E$14="","",E$14)</f>
         <v>x</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="74"/>
-      <c r="B10" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="76" t="s">
+      <c r="A10" s="72"/>
+      <c r="B10" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="D10" s="76" t="s">
+      <c r="D10" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="E10" s="99" t="str">
+      <c r="E10" s="97" t="str">
         <f>IF(E$14="","",E$14)</f>
         <v>x</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="74"/>
-      <c r="B11" s="73" t="s">
+      <c r="A11" s="72"/>
+      <c r="B11" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="99" t="str">
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="97" t="str">
         <f>IF(E$14="","",E$14)</f>
         <v>x</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="74"/>
-      <c r="B12" s="73" t="s">
+      <c r="A12" s="72"/>
+      <c r="B12" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="99" t="str">
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="97" t="str">
         <f>IF(E$14="","",E$14)</f>
         <v>x</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="74"/>
-      <c r="B13" s="73" t="s">
+      <c r="A13" s="72"/>
+      <c r="B13" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="99" t="str">
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="97" t="str">
         <f>IF(E$14="","",E$14)</f>
         <v>x</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="74"/>
-      <c r="B14" s="73" t="s">
+      <c r="A14" s="72"/>
+      <c r="B14" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="76" t="s">
+      <c r="C14" s="70"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="74" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="100" t="str">
+      <c r="C16" s="68"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="98" t="str">
         <f>IF(E$21="","",E$21)</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="74"/>
-      <c r="B17" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="99" t="str">
+      <c r="A17" s="72"/>
+      <c r="B17" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="68"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="97" t="str">
         <f>IF(E$21="","",E$21)</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="74"/>
-      <c r="B18" s="73" t="s">
+      <c r="A18" s="72"/>
+      <c r="B18" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="99" t="str">
+      <c r="C18" s="68"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="97" t="str">
         <f>IF(E$21="","",E$21)</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="74"/>
-      <c r="B19" s="73" t="s">
+      <c r="A19" s="72"/>
+      <c r="B19" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="99" t="str">
+      <c r="C19" s="68"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="97" t="str">
         <f>IF(E$21="","",E$21)</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="74"/>
-      <c r="B20" s="73" t="s">
+      <c r="A20" s="72"/>
+      <c r="B20" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="99" t="str">
+      <c r="C20" s="68"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="97" t="str">
         <f>IF(E$21="","",E$21)</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="74"/>
-      <c r="B21" s="73" t="s">
+      <c r="A21" s="72"/>
+      <c r="B21" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10389,7 +10389,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+    <sheetView zoomScale="175" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -10402,44 +10402,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="79" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="105" t="s">
+      <c r="C1" s="103" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="105" t="s">
+      <c r="D1" s="103" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="71" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="74" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="103" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="71" t="s">
         <v>214</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="74" t="s">
         <v>197</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Plotting for optimized budget multiples, removed spreadsheet from master
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_input.xlsx
+++ b/applications/default/data/national/default_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{518C0E23-D2C4-B344-9720-3F3088D82331}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{773C632A-22D1-5145-92E0-474C1856D341}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="-20740" windowWidth="27100" windowHeight="18820" tabRatio="961" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="-20740" windowWidth="27100" windowHeight="18820" tabRatio="961" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4967,8 +4967,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5412,7 +5412,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="81">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C30" s="81">
         <v>0.95</v>
@@ -5671,7 +5671,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8540,7 +8540,7 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated with Tanzania data
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_input.xlsx
+++ b/applications/default/data/national/default_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{773C632A-22D1-5145-92E0-474C1856D341}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{50E1BEEA-4C3F-3D48-B662-A0DDD12DB3CE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="-20740" windowWidth="27100" windowHeight="18820" tabRatio="961" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="961" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -183,106 +183,6 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>1.5*unit cost of BFP</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>0.5* unit cost of BFP</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Totally fictional</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
       <text>
         <r>
@@ -335,7 +235,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -378,7 +278,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -454,7 +354,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -532,7 +432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="222">
   <si>
     <t>year</t>
   </si>
@@ -904,9 +804,6 @@
   </si>
   <si>
     <t>Percentage of diarrhea that is severe</t>
-  </si>
-  <si>
-    <t>Total population</t>
   </si>
   <si>
     <t>Number of births</t>
@@ -2221,7 +2118,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2430,6 +2327,10 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="727">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -4586,7 +4487,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4601,10 +4502,10 @@
         <v>112</v>
       </c>
       <c r="B1" s="64" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="64" t="s">
         <v>187</v>
-      </c>
-      <c r="C1" s="64" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4617,15 +4518,15 @@
         <v>118</v>
       </c>
       <c r="C3" s="24">
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="23">
-        <v>0.1</v>
+      <c r="C4" s="106">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4633,7 +4534,7 @@
         <v>117</v>
       </c>
       <c r="C5" s="23">
-        <v>0.35199999999999998</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4641,7 +4542,7 @@
         <v>120</v>
       </c>
       <c r="C6" s="24">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4649,7 +4550,7 @@
         <v>121</v>
       </c>
       <c r="C7" s="24">
-        <v>0.3</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4657,7 +4558,7 @@
         <v>122</v>
       </c>
       <c r="C8" s="24">
-        <v>0.1</v>
+        <v>0.221</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4683,7 +4584,7 @@
         <v>107</v>
       </c>
       <c r="C12" s="23">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4691,7 +4592,7 @@
         <v>108</v>
       </c>
       <c r="C13" s="23">
-        <v>0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4699,7 +4600,7 @@
         <v>109</v>
       </c>
       <c r="C14" s="23">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4708,7 +4609,7 @@
       </c>
       <c r="C15" s="26">
         <f>1-frac_rice-frac_wheat-frac_maize</f>
-        <v>2.9999999999999957E-2</v>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4724,7 +4625,7 @@
         <v>113</v>
       </c>
       <c r="C18" s="23">
-        <v>0.29978973218277538</v>
+        <v>0.127</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4732,7 +4633,7 @@
         <v>114</v>
       </c>
       <c r="C19" s="23">
-        <v>0.52556568434139284</v>
+        <v>0.45200000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4740,7 +4641,7 @@
         <v>115</v>
       </c>
       <c r="C20" s="23">
-        <v>0.16210210664201097</v>
+        <v>0.33400000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4748,13 +4649,13 @@
         <v>116</v>
       </c>
       <c r="C21" s="23">
-        <v>1.2542476833820825E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4769,7 +4670,7 @@
         <v>104</v>
       </c>
       <c r="C25" s="25">
-        <v>25.4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4777,7 +4678,7 @@
         <v>103</v>
       </c>
       <c r="C26" s="25">
-        <v>34.68</v>
+        <v>43</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
@@ -4787,17 +4688,17 @@
         <v>102</v>
       </c>
       <c r="C27" s="25">
-        <v>39.32</v>
+        <v>67</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C28" s="25">
-        <v>1.76</v>
+        <v>4.01</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4813,7 +4714,7 @@
         <v>105</v>
       </c>
       <c r="C30" s="25">
-        <v>25.36</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4821,7 +4722,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D32" s="20"/>
     </row>
@@ -4875,48 +4776,48 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C39" s="7">
-        <v>2.4300000000000002</v>
+        <v>1.66</v>
       </c>
       <c r="D39" s="20"/>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C40" s="7">
-        <v>2.4300000000000002</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="7">
-        <v>3.71</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C42" s="7">
-        <v>3</v>
+        <v>5.43</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C43" s="7">
-        <v>1.92</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4929,7 +4830,7 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C47" s="24">
         <v>0.42</v>
@@ -4937,7 +4838,7 @@
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C48" s="24">
         <v>1</v>
@@ -4945,7 +4846,7 @@
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C49" s="24">
         <v>1</v>
@@ -4967,8 +4868,8 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4985,13 +4886,13 @@
         <v>70</v>
       </c>
       <c r="B1" s="90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C1" s="89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D1" s="88" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5043,7 +4944,7 @@
         <v>61</v>
       </c>
       <c r="B5" s="81">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="81">
         <v>0.95</v>
@@ -5059,7 +4960,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="81">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C6" s="81">
         <v>0.95</v>
@@ -5075,13 +4976,13 @@
         <v>63</v>
       </c>
       <c r="B7" s="81">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="C7" s="81">
         <v>0.95</v>
       </c>
       <c r="D7" s="82">
-        <v>0.14000000000000001</v>
+        <v>25</v>
       </c>
       <c r="E7" s="85"/>
     </row>
@@ -5117,7 +5018,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B10" s="81">
         <v>0</v>
@@ -5131,7 +5032,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" s="81">
         <v>0</v>
@@ -5145,7 +5046,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="101" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="81">
         <v>0</v>
@@ -5159,7 +5060,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="101" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" s="81">
         <v>0</v>
@@ -5173,7 +5074,7 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B14" s="81">
         <v>0</v>
@@ -5187,7 +5088,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B15" s="81">
         <v>0</v>
@@ -5204,7 +5105,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="81">
-        <v>0</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="C16" s="81">
         <v>0.95</v>
@@ -5219,19 +5120,19 @@
         <v>47</v>
       </c>
       <c r="B17" s="81">
-        <v>0</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="C17" s="81">
         <v>0.95</v>
       </c>
       <c r="D17" s="82">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="E17" s="67"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" s="81">
         <v>0</v>
@@ -5241,12 +5142,12 @@
       </c>
       <c r="D18" s="100">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
-        <v>1.22</v>
+        <v>10.49</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B19" s="81">
         <v>0</v>
@@ -5256,12 +5157,12 @@
       </c>
       <c r="D19" s="100">
         <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$9:$E$13&lt;&gt;""))</f>
-        <v>1.4700000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20" s="81">
         <v>0</v>
@@ -5276,7 +5177,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B21" s="81">
         <v>0</v>
@@ -5294,7 +5195,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="81">
-        <v>0.2</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C22" s="81">
         <v>0.95</v>
@@ -5336,16 +5237,16 @@
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B25" s="81">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C25" s="81">
         <v>0.95</v>
       </c>
       <c r="D25" s="82">
-        <v>1</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="E25" s="67"/>
     </row>
@@ -5354,13 +5255,13 @@
         <v>59</v>
       </c>
       <c r="B26" s="81">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="C26" s="81">
         <v>0.95</v>
       </c>
       <c r="D26" s="82">
-        <v>2.99</v>
+        <v>3.78</v>
       </c>
       <c r="E26" s="67"/>
     </row>
@@ -5404,7 +5305,7 @@
       </c>
       <c r="D29" s="83">
         <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
-        <v>23.363600000000005</v>
+        <v>10.015195269175592</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5412,13 +5313,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="81">
-        <v>0.6</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="C30" s="81">
         <v>0.95</v>
       </c>
       <c r="D30" s="82">
-        <v>0.35</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5426,13 +5327,13 @@
         <v>94</v>
       </c>
       <c r="B31" s="81">
-        <v>0</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C31" s="81">
         <v>0.95</v>
       </c>
       <c r="D31" s="82">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5440,13 +5341,13 @@
         <v>93</v>
       </c>
       <c r="B32" s="81">
-        <v>0</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="C32" s="81">
         <v>0.95</v>
       </c>
       <c r="D32" s="82">
-        <v>2.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5454,13 +5355,13 @@
         <v>92</v>
       </c>
       <c r="B33" s="81">
-        <v>0</v>
+        <v>0.316</v>
       </c>
       <c r="C33" s="81">
         <v>0.95</v>
       </c>
       <c r="D33" s="82">
-        <v>50.26</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5468,13 +5369,13 @@
         <v>90</v>
       </c>
       <c r="B34" s="81">
-        <v>0</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="C34" s="81">
         <v>0.95</v>
       </c>
       <c r="D34" s="82">
-        <v>36.1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5482,13 +5383,13 @@
         <v>91</v>
       </c>
       <c r="B35" s="81">
-        <v>0</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="C35" s="81">
         <v>0.95</v>
       </c>
       <c r="D35" s="82">
-        <v>231.85</v>
+        <v>102</v>
       </c>
       <c r="F35" s="58"/>
     </row>
@@ -5497,13 +5398,13 @@
         <v>96</v>
       </c>
       <c r="B36" s="81">
-        <v>0</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="C36" s="81">
         <v>0.95</v>
       </c>
       <c r="D36" s="82">
-        <v>1.5</v>
+        <v>5.53</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5534,14 +5435,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5552,24 +5453,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A1" s="96" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="95" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C1" s="95" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D1" s="95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E1" s="95" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="94" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="93" t="s">
         <v>32</v>
@@ -5579,8 +5480,7 @@
         <v>0.91500000000000004</v>
       </c>
       <c r="D2" s="82">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
+        <v>3.78</v>
       </c>
       <c r="E2" s="82">
         <v>0.05</v>
@@ -5596,8 +5496,8 @@
         <v>0.91500000000000004</v>
       </c>
       <c r="D3" s="82">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
+        <f t="shared" ref="D3:D6" si="0">10.49/4</f>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E3" s="82">
         <v>0.05</v>
@@ -5613,8 +5513,8 @@
         <v>0.91500000000000004</v>
       </c>
       <c r="D4" s="82">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
+        <f t="shared" si="0"/>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E4" s="82">
         <v>0.05</v>
@@ -5630,8 +5530,8 @@
         <v>0.91500000000000004</v>
       </c>
       <c r="D5" s="82">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
+        <f t="shared" si="0"/>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E5" s="82">
         <v>0.05</v>
@@ -5647,8 +5547,8 @@
         <v>0.91500000000000004</v>
       </c>
       <c r="D6" s="82">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
+        <f t="shared" si="0"/>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E6" s="82">
         <v>0.05</v>
@@ -5659,7 +5559,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5687,15 +5586,15 @@
         <v>70</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="74" t="s">
         <v>59</v>
@@ -5704,7 +5603,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="74" t="s">
         <v>59</v>
@@ -5716,16 +5615,16 @@
         <v>58</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="74"/>
     </row>
@@ -5866,7 +5765,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5897,23 +5796,23 @@
       </c>
       <c r="B2" s="37">
         <f>'Baseline year population inputs'!C39</f>
-        <v>2.4300000000000002</v>
+        <v>1.66</v>
       </c>
       <c r="C2" s="37">
         <f>'Baseline year population inputs'!C40</f>
-        <v>2.4300000000000002</v>
+        <v>1.66</v>
       </c>
       <c r="D2" s="37">
         <f>'Baseline year population inputs'!C41</f>
-        <v>3.71</v>
+        <v>5.64</v>
       </c>
       <c r="E2" s="37">
         <f>'Baseline year population inputs'!C42</f>
-        <v>3</v>
+        <v>5.43</v>
       </c>
       <c r="F2" s="37">
         <f>'Baseline year population inputs'!C43</f>
-        <v>1.92</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5922,23 +5821,23 @@
       </c>
       <c r="B3" s="37">
         <f>frac_mam_1month * 2.6</f>
-        <v>0.39</v>
+        <v>0.1404</v>
       </c>
       <c r="C3" s="37">
         <f>frac_mam_1_5months * 2.6</f>
-        <v>0.39</v>
+        <v>0.1404</v>
       </c>
       <c r="D3" s="37">
         <f>frac_mam_6_11months * 2.6</f>
-        <v>0.33540000000000003</v>
+        <v>0.14045866666666668</v>
       </c>
       <c r="E3" s="37">
         <f>frac_mam_12_23months * 2.6</f>
-        <v>0.28600000000000003</v>
+        <v>0.11062404115996258</v>
       </c>
       <c r="F3" s="37">
         <f>frac_mam_24_59months * 2.6</f>
-        <v>0.27300000000000002</v>
+        <v>5.8059717622450747E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5947,23 +5846,23 @@
       </c>
       <c r="B4" s="37">
         <f>frac_sam_1month * 2.6</f>
-        <v>0.12740000000000001</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="C4" s="37">
         <f>frac_sam_1_5months * 2.6</f>
-        <v>0.12740000000000001</v>
+        <v>0.10400000000000001</v>
       </c>
       <c r="D4" s="37">
         <f>frac_sam_6_11months * 2.6</f>
-        <v>0.13780000000000001</v>
+        <v>4.0885333333333343E-2</v>
       </c>
       <c r="E4" s="37">
         <f>frac_sam_12_23months * 2.6</f>
-        <v>0.10659999999999999</v>
+        <v>2.6248082319925165E-2</v>
       </c>
       <c r="F4" s="37">
         <f>frac_sam_24_59months * 2.6</f>
-        <v>5.4600000000000003E-2</v>
+        <v>1.9069687990238803E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6055,19 +5954,19 @@
       </c>
       <c r="D2" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="E2" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="F2" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="G2" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="H2" s="55">
         <v>0</v>
@@ -6096,7 +5995,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" s="57">
         <v>1</v>
@@ -6140,7 +6039,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="54">
         <v>0</v>
@@ -6150,11 +6049,11 @@
       </c>
       <c r="E4" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="F4" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="G4" s="54">
         <v>0</v>
@@ -6186,7 +6085,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="54">
         <v>0</v>
@@ -6287,11 +6186,11 @@
       </c>
       <c r="E7" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="F7" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="G7" s="54">
         <v>0</v>
@@ -6528,19 +6427,19 @@
       </c>
       <c r="H13" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="I13" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="J13" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="K13" s="54">
         <f>food_insecure</f>
-        <v>0.36</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="L13" s="55">
         <v>0</v>
@@ -6603,7 +6502,7 @@
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" s="55">
         <v>0</v>
@@ -6652,7 +6551,7 @@
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C16" s="55">
         <v>0</v>
@@ -6671,19 +6570,19 @@
       </c>
       <c r="H16" s="54">
         <f>frac_PW_health_facility</f>
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="I16" s="54">
         <f>frac_PW_health_facility</f>
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="J16" s="54">
         <f>frac_PW_health_facility</f>
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="K16" s="54">
         <f>frac_PW_health_facility</f>
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="L16" s="55">
         <v>0</v>
@@ -6719,19 +6618,19 @@
       </c>
       <c r="H17" s="54">
         <f>frac_malaria_risk</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I17" s="54">
         <f>frac_malaria_risk</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J17" s="54">
         <f>frac_malaria_risk</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="K17" s="54">
         <f>frac_malaria_risk</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="L17" s="55">
         <v>0</v>
@@ -6978,7 +6877,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C24" s="55">
         <v>0</v>
@@ -7009,24 +6908,24 @@
       </c>
       <c r="L24" s="54">
         <f>(1-food_insecure)*(0.49)*(1-school_attendance) + food_insecure*(0.7)*(1-school_attendance)</f>
-        <v>0.36650879999999997</v>
+        <v>0.42289939999999993</v>
       </c>
       <c r="M24" s="54">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
-        <v>0.56559999999999999</v>
+        <v>0.54921999999999993</v>
       </c>
       <c r="N24" s="54">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
-        <v>0.56559999999999999</v>
+        <v>0.54921999999999993</v>
       </c>
       <c r="O24" s="54">
         <f>(1-food_insecure)*(0.49)+food_insecure*(0.7)</f>
-        <v>0.56559999999999999</v>
+        <v>0.54921999999999993</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C25" s="55">
         <v>0</v>
@@ -7057,24 +6956,24 @@
       </c>
       <c r="L25" s="54">
         <f>(1-food_insecure)*(0.21)*(1-school_attendance) + food_insecure*(0.3)*(1-school_attendance)</f>
-        <v>0.1570752</v>
+        <v>0.18124259999999998</v>
       </c>
       <c r="M25" s="54">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
-        <v>0.2424</v>
+        <v>0.23537999999999998</v>
       </c>
       <c r="N25" s="54">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
-        <v>0.2424</v>
+        <v>0.23537999999999998</v>
       </c>
       <c r="O25" s="54">
         <f>(1-food_insecure)*(0.21)+food_insecure*(0.3)</f>
-        <v>0.2424</v>
+        <v>0.23537999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="101" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C26" s="55">
         <v>0</v>
@@ -7105,24 +7004,24 @@
       </c>
       <c r="L26" s="54">
         <f>(1-food_insecure)*(0.3)*(1-school_attendance)</f>
-        <v>0.12441600000000001</v>
+        <v>0.16585799999999998</v>
       </c>
       <c r="M26" s="54">
         <f>(1-food_insecure)*(0.3)</f>
-        <v>0.192</v>
+        <v>0.21539999999999998</v>
       </c>
       <c r="N26" s="54">
         <f>(1-food_insecure)*(0.3)</f>
-        <v>0.192</v>
+        <v>0.21539999999999998</v>
       </c>
       <c r="O26" s="54">
         <f>(1-food_insecure)*(0.3)</f>
-        <v>0.192</v>
+        <v>0.21539999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="101" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C27" s="55">
         <v>0</v>
@@ -7153,7 +7052,7 @@
       </c>
       <c r="L27" s="54">
         <f>(1-food_insecure)*1*school_attendance + food_insecure*1*school_attendance</f>
-        <v>0.35199999999999998</v>
+        <v>0.23</v>
       </c>
       <c r="M27" s="54">
         <v>0</v>
@@ -7190,47 +7089,47 @@
       </c>
       <c r="E29" s="54">
         <f t="shared" ref="E29:O29" si="0">frac_maize</f>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="F29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="G29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="H29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="I29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="J29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="K29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="L29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="M29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="N29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="O29" s="54">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7245,47 +7144,47 @@
       </c>
       <c r="E30" s="54">
         <f t="shared" ref="E30:O30" si="1">frac_rice</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="K30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="N30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="O30" s="54">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7300,47 +7199,47 @@
       </c>
       <c r="E31" s="54">
         <f t="shared" ref="E31:O31" si="2">frac_wheat</f>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="F31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="G31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="H31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="I31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="J31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="K31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="L31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="M31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="N31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="O31" s="54">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7393,55 +7292,55 @@
       </c>
       <c r="C33" s="54">
         <f t="shared" ref="C33:O33" si="3">frac_malaria_risk</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="K33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="L33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="O33" s="54">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7700,24 +7599,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D1" s="63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="61">
         <v>0.9</v>
@@ -7735,7 +7634,7 @@
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="61">
         <v>1</v>
@@ -7753,7 +7652,7 @@
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="61">
         <v>1</v>
@@ -7771,7 +7670,7 @@
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="62" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B5" s="61">
         <v>1</v>
@@ -7789,7 +7688,7 @@
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B6" s="61">
         <v>1</v>
@@ -7807,7 +7706,7 @@
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="62" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7" s="61">
         <v>0.93</v>
@@ -7825,7 +7724,7 @@
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" s="61">
         <v>0.5</v>
@@ -7843,7 +7742,7 @@
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" s="61">
         <v>0.5</v>
@@ -7861,7 +7760,7 @@
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="62" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="61">
         <v>0.98</v>
@@ -7895,7 +7794,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7906,7 +7805,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>1</v>
@@ -7932,7 +7831,7 @@
         <v>74</v>
       </c>
       <c r="B2" s="33">
-        <v>7.0000000000000001E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="C2" s="34">
         <v>0</v>
@@ -7955,7 +7854,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="33">
-        <v>0.19900000000000001</v>
+        <v>0.1966</v>
       </c>
       <c r="C3" s="34">
         <v>0</v>
@@ -7978,7 +7877,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="33">
-        <v>5.8999999999999997E-2</v>
+        <v>6.2100000000000002E-2</v>
       </c>
       <c r="C4" s="34">
         <v>0</v>
@@ -8001,7 +7900,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="33">
-        <v>0.22900000000000001</v>
+        <v>0.29289999999999999</v>
       </c>
       <c r="C5" s="34">
         <v>0</v>
@@ -8024,7 +7923,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="33">
-        <v>0.29699999999999999</v>
+        <v>0.24709999999999999</v>
       </c>
       <c r="C6" s="34">
         <v>0</v>
@@ -8047,7 +7946,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="33">
-        <v>6.0000000000000001E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="C7" s="34">
         <v>0</v>
@@ -8070,7 +7969,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="33">
-        <v>0.127</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="C8" s="34">
         <v>0</v>
@@ -8093,7 +7992,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="33">
-        <v>7.5999999999999998E-2</v>
+        <v>6.1800000000000001E-2</v>
       </c>
       <c r="C9" s="34">
         <v>0</v>
@@ -8119,17 +8018,16 @@
         <v>0</v>
       </c>
       <c r="C10" s="33">
-        <f>14.81% * 0.2</f>
-        <v>2.9620000000000004E-2</v>
+        <v>0.1368</v>
       </c>
       <c r="D10" s="33">
-        <v>0.14810000000000001</v>
+        <v>0.1368</v>
       </c>
       <c r="E10" s="33">
-        <v>0.14810000000000001</v>
+        <v>0.1368</v>
       </c>
       <c r="F10" s="33">
-        <v>0.14810000000000001</v>
+        <v>0.1368</v>
       </c>
       <c r="G10" s="34">
         <v>0</v>
@@ -8143,16 +8041,16 @@
         <v>0</v>
       </c>
       <c r="C11" s="33">
-        <v>0.2883</v>
+        <v>0.20660000000000001</v>
       </c>
       <c r="D11" s="33">
-        <v>0.2883</v>
+        <v>0.20660000000000001</v>
       </c>
       <c r="E11" s="33">
-        <v>0.2883</v>
+        <v>0.20660000000000001</v>
       </c>
       <c r="F11" s="33">
-        <v>0.2883</v>
+        <v>0.20660000000000001</v>
       </c>
       <c r="G11" s="34">
         <v>0</v>
@@ -8166,16 +8064,16 @@
         <v>0</v>
       </c>
       <c r="C12" s="33">
-        <v>4.1000000000000002E-2</v>
+        <v>2.1100000000000001E-2</v>
       </c>
       <c r="D12" s="33">
-        <v>4.1000000000000002E-2</v>
+        <v>2.1100000000000001E-2</v>
       </c>
       <c r="E12" s="33">
-        <v>4.1000000000000002E-2</v>
+        <v>2.1100000000000001E-2</v>
       </c>
       <c r="F12" s="33">
-        <v>4.1000000000000002E-2</v>
+        <v>2.1100000000000001E-2</v>
       </c>
       <c r="G12" s="34">
         <v>0</v>
@@ -8189,16 +8087,16 @@
         <v>0</v>
       </c>
       <c r="C13" s="33">
-        <v>5.0099999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="D13" s="33">
-        <v>5.0099999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E13" s="33">
-        <v>5.0099999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="F13" s="33">
-        <v>5.0099999999999999E-2</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="G13" s="34">
         <v>0</v>
@@ -8212,16 +8110,16 @@
         <v>0</v>
       </c>
       <c r="C14" s="33">
-        <v>6.0000000000000001E-3</v>
+        <v>8.6199999999999999E-2</v>
       </c>
       <c r="D14" s="33">
-        <v>6.0000000000000001E-3</v>
+        <v>8.6199999999999999E-2</v>
       </c>
       <c r="E14" s="33">
-        <v>6.0000000000000001E-3</v>
+        <v>8.6199999999999999E-2</v>
       </c>
       <c r="F14" s="33">
-        <v>6.0000000000000001E-3</v>
+        <v>8.6199999999999999E-2</v>
       </c>
       <c r="G14" s="34">
         <v>0</v>
@@ -8235,16 +8133,16 @@
         <v>0</v>
       </c>
       <c r="C15" s="33">
-        <v>0.01</v>
+        <v>2.86E-2</v>
       </c>
       <c r="D15" s="33">
-        <v>0.01</v>
+        <v>2.86E-2</v>
       </c>
       <c r="E15" s="33">
-        <v>0.01</v>
+        <v>2.86E-2</v>
       </c>
       <c r="F15" s="33">
-        <v>0.01</v>
+        <v>2.86E-2</v>
       </c>
       <c r="G15" s="34">
         <v>0</v>
@@ -8258,16 +8156,16 @@
         <v>0</v>
       </c>
       <c r="C16" s="33">
-        <v>0</v>
+        <v>1.5299999999999999E-2</v>
       </c>
       <c r="D16" s="33">
-        <v>0</v>
+        <v>1.5299999999999999E-2</v>
       </c>
       <c r="E16" s="33">
-        <v>0</v>
+        <v>1.5299999999999999E-2</v>
       </c>
       <c r="F16" s="33">
-        <v>0</v>
+        <v>1.5299999999999999E-2</v>
       </c>
       <c r="G16" s="34">
         <v>0</v>
@@ -8281,16 +8179,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="33">
-        <v>0.14510000000000001</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="D17" s="33">
-        <v>0.14510000000000001</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="E17" s="33">
-        <v>0.14510000000000001</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="F17" s="33">
-        <v>0.14510000000000001</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="G17" s="34">
         <v>0</v>
@@ -8304,16 +8202,16 @@
         <v>0</v>
       </c>
       <c r="C18" s="33">
-        <v>0.31130000000000002</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="D18" s="33">
-        <v>0.31130000000000002</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="E18" s="33">
-        <v>0.31130000000000002</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="F18" s="33">
-        <v>0.31130000000000002</v>
+        <v>0.36199999999999999</v>
       </c>
       <c r="G18" s="34">
         <v>0</v>
@@ -8339,7 +8237,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="35">
-        <v>2.5899999999999999E-2</v>
+        <v>0.10082724000000001</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8362,7 +8260,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="35">
-        <v>7.1000000000000004E-3</v>
+        <v>3.1206000000000002E-4</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8385,7 +8283,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="35">
-        <v>0.25590000000000002</v>
+        <v>0.15891214000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8408,7 +8306,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="35">
-        <v>0.1464</v>
+        <v>0.12598688999999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8431,7 +8329,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="35">
-        <v>1.7600000000000001E-2</v>
+        <v>0.12434007</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8454,7 +8352,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="35">
-        <v>1.8100000000000002E-2</v>
+        <v>3.9028409999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8477,7 +8375,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="35">
-        <v>1.14E-2</v>
+        <v>8.5254999999999999E-4</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8500,7 +8398,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="35">
-        <v>0.15129999999999999</v>
+        <v>6.8467810000000004E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8523,7 +8421,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="35">
-        <v>0.36630000000000001</v>
+        <v>0.38127283000000001</v>
       </c>
     </row>
   </sheetData>
@@ -8538,30 +8436,30 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
-    <col min="2" max="10" width="16.83203125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" style="15" customWidth="1"/>
-    <col min="13" max="16384" width="14.5" style="15"/>
+    <col min="2" max="9" width="16.83203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="14.5" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>125</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>126</v>
       </c>
       <c r="D1" s="31" t="s">
         <v>49</v>
@@ -8576,607 +8474,562 @@
         <v>52</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="K1" s="104" t="s">
         <v>149</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="J1" s="104" t="s">
+        <v>148</v>
+      </c>
+      <c r="K1" s="31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9">
         <v>2017</v>
       </c>
       <c r="B2" s="8">
-        <v>3095470</v>
+        <v>2110000</v>
       </c>
       <c r="C2" s="29">
-        <v>15402200</v>
+        <v>9862402</v>
       </c>
       <c r="D2" s="29">
-        <v>8785700</v>
+        <v>3032037</v>
       </c>
       <c r="E2" s="29">
-        <v>13889200</v>
+        <v>4756743</v>
       </c>
       <c r="F2" s="29">
-        <v>12671800</v>
+        <v>3406589</v>
       </c>
       <c r="G2" s="29">
-        <v>9362400</v>
-      </c>
-      <c r="H2" s="29">
-        <v>173766200</v>
+        <v>2174712</v>
+      </c>
+      <c r="H2" s="30">
+        <f>D2+E2+F2+G2</f>
+        <v>13370081</v>
       </c>
       <c r="I2" s="30">
-        <f t="shared" ref="I2:I15" si="0">D2+E2+F2+G2</f>
-        <v>44709100</v>
-      </c>
-      <c r="J2" s="30">
-        <f t="shared" ref="J2:J15" si="1">(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
-        <v>3650590.4685349194</v>
-      </c>
-      <c r="K2" s="105">
-        <f t="shared" ref="K2:K15" si="2">D2/I2</f>
-        <v>0.19650809343064388</v>
-      </c>
-      <c r="L2" s="30">
-        <f>I2-J2</f>
-        <v>41058509.531465083</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
+        <v>2480858.588708919</v>
+      </c>
+      <c r="J2" s="105">
+        <f>D2/H2</f>
+        <v>0.22677775848927167</v>
+      </c>
+      <c r="K2" s="30">
+        <f>H2-I2</f>
+        <v>10889222.411291081</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9">
         <v>2018</v>
       </c>
       <c r="B3" s="8">
-        <v>3071259</v>
+        <v>2150000</v>
       </c>
       <c r="C3" s="29">
-        <v>15629400.000000002</v>
+        <v>10050371</v>
       </c>
       <c r="D3" s="29">
-        <v>8937400.0000000019</v>
+        <v>3164674</v>
       </c>
       <c r="E3" s="29">
-        <v>14228400.000000002</v>
+        <v>4882700</v>
       </c>
       <c r="F3" s="29">
-        <v>12949600</v>
+        <v>3520083</v>
       </c>
       <c r="G3" s="29">
-        <v>9576800</v>
-      </c>
-      <c r="H3" s="29">
-        <v>175848400</v>
+        <v>2275309</v>
+      </c>
+      <c r="H3" s="30">
+        <f>D3+E3+F3+G3</f>
+        <v>13842766</v>
       </c>
       <c r="I3" s="30">
-        <f t="shared" si="0"/>
-        <v>45692200</v>
-      </c>
-      <c r="J3" s="30">
-        <f t="shared" si="1"/>
-        <v>3622037.632993402</v>
-      </c>
-      <c r="K3" s="105">
-        <f t="shared" si="2"/>
-        <v>0.19560012431005733</v>
-      </c>
-      <c r="L3" s="30">
-        <f t="shared" ref="L3:L15" si="3">I3-J3</f>
-        <v>42070162.3670066</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
+        <v>2527889.0832815999</v>
+      </c>
+      <c r="J3" s="105">
+        <f>D3/H3</f>
+        <v>0.22861572607671038</v>
+      </c>
+      <c r="K3" s="30">
+        <f t="shared" ref="K3:K15" si="0">H3-I3</f>
+        <v>11314876.916718401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9">
         <v>2019</v>
       </c>
       <c r="B4" s="8">
-        <v>3045241</v>
+        <v>2200000</v>
       </c>
       <c r="C4" s="29">
-        <v>15856600.000000002</v>
+        <v>10237786</v>
       </c>
       <c r="D4" s="29">
-        <v>9089100.0000000019</v>
+        <v>3296354</v>
       </c>
       <c r="E4" s="29">
-        <v>14567600.000000002</v>
+        <v>5018666</v>
       </c>
       <c r="F4" s="29">
-        <v>13227400</v>
+        <v>3634703</v>
       </c>
       <c r="G4" s="29">
-        <v>9791200.0000000019</v>
-      </c>
-      <c r="H4" s="29">
-        <v>177930600</v>
+        <v>2379017</v>
+      </c>
+      <c r="H4" s="30">
+        <f>D4+E4+F4+G4</f>
+        <v>14328740</v>
       </c>
       <c r="I4" s="30">
+        <f>(B4 + stillbirth*B4/(1000-stillbirth))/(1-abortion)</f>
+        <v>2586677.2014974509</v>
+      </c>
+      <c r="J4" s="105">
+        <f>D4/H4</f>
+        <v>0.23005190965849057</v>
+      </c>
+      <c r="K4" s="30">
         <f t="shared" si="0"/>
-        <v>46675300</v>
-      </c>
-      <c r="J4" s="30">
-        <f t="shared" si="1"/>
-        <v>3591353.7424015561</v>
-      </c>
-      <c r="K4" s="105">
-        <f t="shared" si="2"/>
-        <v>0.19473040344679096</v>
-      </c>
-      <c r="L4" s="30">
-        <f t="shared" si="3"/>
-        <v>43083946.257598445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>11742062.79850255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>2020</v>
       </c>
       <c r="B5" s="8">
-        <v>3017266</v>
+        <v>2240000</v>
       </c>
       <c r="C5" s="29">
-        <v>16083800.000000004</v>
+        <v>10438537</v>
       </c>
       <c r="D5" s="29">
-        <v>9240800.0000000037</v>
+        <v>3418969</v>
       </c>
       <c r="E5" s="29">
-        <v>14906800.000000004</v>
+        <v>5168014</v>
       </c>
       <c r="F5" s="29">
-        <v>13505200</v>
+        <v>3750324</v>
       </c>
       <c r="G5" s="29">
-        <v>10005600.000000004</v>
-      </c>
-      <c r="H5" s="29">
-        <v>180012800</v>
+        <v>2484409</v>
+      </c>
+      <c r="H5" s="30">
+        <f>D5+E5+F5+G5</f>
+        <v>14821716</v>
       </c>
       <c r="I5" s="30">
+        <f>(B5 + stillbirth*B5/(1000-stillbirth))/(1-abortion)</f>
+        <v>2633707.6960701318</v>
+      </c>
+      <c r="J5" s="105">
+        <f>D5/H5</f>
+        <v>0.23067295311824892</v>
+      </c>
+      <c r="K5" s="30">
         <f t="shared" si="0"/>
-        <v>47658400.000000015</v>
-      </c>
-      <c r="J5" s="30">
-        <f t="shared" si="1"/>
-        <v>3558361.8967828737</v>
-      </c>
-      <c r="K5" s="105">
-        <f t="shared" si="2"/>
-        <v>0.19389656387960991</v>
-      </c>
-      <c r="L5" s="30">
-        <f t="shared" si="3"/>
-        <v>44100038.10321714</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>12188008.303929869</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>2021</v>
       </c>
       <c r="B6" s="8">
-        <v>2990677</v>
+        <v>2280000</v>
       </c>
       <c r="C6" s="29">
-        <v>16311000.000000004</v>
+        <v>10636534</v>
       </c>
       <c r="D6" s="29">
-        <v>9392500.0000000037</v>
+        <v>3532758</v>
       </c>
       <c r="E6" s="29">
-        <v>15246000.000000004</v>
+        <v>5332455</v>
       </c>
       <c r="F6" s="29">
-        <v>13783000</v>
+        <v>3869436</v>
       </c>
       <c r="G6" s="29">
-        <v>10220000.000000004</v>
-      </c>
-      <c r="H6" s="29">
-        <v>182095000</v>
+        <v>2592003</v>
+      </c>
+      <c r="H6" s="30">
+        <f>D6+E6+F6+G6</f>
+        <v>15326652</v>
       </c>
       <c r="I6" s="30">
+        <f>(B6 + stillbirth*B6/(1000-stillbirth))/(1-abortion)</f>
+        <v>2680738.1906428128</v>
+      </c>
+      <c r="J6" s="105">
+        <f>D6/H6</f>
+        <v>0.23049769773594389</v>
+      </c>
+      <c r="K6" s="30">
         <f t="shared" si="0"/>
-        <v>48641500.000000015</v>
-      </c>
-      <c r="J6" s="30">
-        <f t="shared" si="1"/>
-        <v>3527004.6069471212</v>
-      </c>
-      <c r="K6" s="105">
-        <f t="shared" si="2"/>
-        <v>0.1930964300031866</v>
-      </c>
-      <c r="L6" s="30">
-        <f t="shared" si="3"/>
-        <v>45114495.393052891</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>12645913.809357187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>2022</v>
       </c>
       <c r="B7" s="8">
-        <v>2962144</v>
+        <v>2330000</v>
       </c>
       <c r="C7" s="29">
-        <v>16190600.000000004</v>
+        <v>10854967</v>
       </c>
       <c r="D7" s="29">
-        <v>9004300.0000000037</v>
+        <v>3637390</v>
       </c>
       <c r="E7" s="29">
-        <v>15785700.000000004</v>
+        <v>5508952</v>
       </c>
       <c r="F7" s="29">
-        <v>13711700</v>
+        <v>3990560</v>
       </c>
       <c r="G7" s="29">
-        <v>10609600.000000004</v>
-      </c>
-      <c r="H7" s="29">
-        <v>183822800</v>
+        <v>2701259</v>
+      </c>
+      <c r="H7" s="30">
+        <f>D7+E7+F7+G7</f>
+        <v>15838161</v>
       </c>
       <c r="I7" s="30">
+        <f>(B7 + stillbirth*B7/(1000-stillbirth))/(1-abortion)</f>
+        <v>2739526.3088586638</v>
+      </c>
+      <c r="J7" s="105">
+        <f>D7/H7</f>
+        <v>0.22965987023367171</v>
+      </c>
+      <c r="K7" s="30">
         <f t="shared" si="0"/>
-        <v>49111300.000000015</v>
-      </c>
-      <c r="J7" s="30">
-        <f t="shared" si="1"/>
-        <v>3493354.6934158299</v>
-      </c>
-      <c r="K7" s="105">
-        <f t="shared" si="2"/>
-        <v>0.1833447699409301</v>
-      </c>
-      <c r="L7" s="30">
-        <f t="shared" si="3"/>
-        <v>45617945.306584187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>13098634.691141337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>2023</v>
       </c>
       <c r="B8" s="8">
-        <v>2931643</v>
+        <v>2380000</v>
       </c>
       <c r="C8" s="29">
-        <v>16070200.000000004</v>
+        <v>11089897</v>
       </c>
       <c r="D8" s="29">
-        <v>8616100.0000000019</v>
+        <v>3737403</v>
       </c>
       <c r="E8" s="29">
-        <v>16325400.000000004</v>
+        <v>5696990</v>
       </c>
       <c r="F8" s="29">
-        <v>13640400</v>
+        <v>4112898</v>
       </c>
       <c r="G8" s="29">
-        <v>10999200.000000002</v>
-      </c>
-      <c r="H8" s="29">
-        <v>185550600</v>
+        <v>2811667</v>
+      </c>
+      <c r="H8" s="30">
+        <f>D8+E8+F8+G8</f>
+        <v>16358958</v>
       </c>
       <c r="I8" s="30">
+        <f>(B8 + stillbirth*B8/(1000-stillbirth))/(1-abortion)</f>
+        <v>2798314.4270745148</v>
+      </c>
+      <c r="J8" s="105">
+        <f>D8/H8</f>
+        <v>0.22846216733364069</v>
+      </c>
+      <c r="K8" s="30">
         <f t="shared" si="0"/>
-        <v>49581100.000000007</v>
-      </c>
-      <c r="J8" s="30">
-        <f t="shared" si="1"/>
-        <v>3457383.8521927581</v>
-      </c>
-      <c r="K8" s="105">
-        <f t="shared" si="2"/>
-        <v>0.17377791134121673</v>
-      </c>
-      <c r="L8" s="30">
-        <f t="shared" si="3"/>
-        <v>46123716.147807248</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>13560643.572925486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>2024</v>
       </c>
       <c r="B9" s="8">
-        <v>2899255</v>
+        <v>2420000</v>
       </c>
       <c r="C9" s="29">
-        <v>15949800.000000006</v>
+        <v>11331595</v>
       </c>
       <c r="D9" s="29">
-        <v>8227900.0000000019</v>
+        <v>3840674</v>
       </c>
       <c r="E9" s="29">
-        <v>16865100.000000004</v>
+        <v>5895615</v>
       </c>
       <c r="F9" s="29">
-        <v>13569100</v>
+        <v>4235117</v>
       </c>
       <c r="G9" s="29">
-        <v>11388800</v>
-      </c>
-      <c r="H9" s="29">
-        <v>187278400</v>
+        <v>2922818</v>
+      </c>
+      <c r="H9" s="30">
+        <f>D9+E9+F9+G9</f>
+        <v>16894224</v>
       </c>
       <c r="I9" s="30">
+        <f>(B9 + stillbirth*B9/(1000-stillbirth))/(1-abortion)</f>
+        <v>2845344.9216471957</v>
+      </c>
+      <c r="J9" s="105">
+        <f>D9/H9</f>
+        <v>0.22733651453893355</v>
+      </c>
+      <c r="K9" s="30">
         <f t="shared" si="0"/>
-        <v>50050900.000000007</v>
-      </c>
-      <c r="J9" s="30">
-        <f t="shared" si="1"/>
-        <v>3419187.609265219</v>
-      </c>
-      <c r="K9" s="105">
-        <f t="shared" si="2"/>
-        <v>0.16439065031797631</v>
-      </c>
-      <c r="L9" s="30">
-        <f t="shared" si="3"/>
-        <v>46631712.390734792</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>14048879.078352805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>2025</v>
       </c>
       <c r="B10" s="8">
-        <v>2865008</v>
+        <v>2480000</v>
       </c>
       <c r="C10" s="29">
-        <v>15829400.000000006</v>
+        <v>11574198</v>
       </c>
       <c r="D10" s="29">
-        <v>7839700.0000000019</v>
+        <v>3951644</v>
       </c>
       <c r="E10" s="29">
-        <v>17404800.000000004</v>
+        <v>6103745</v>
       </c>
       <c r="F10" s="29">
-        <v>13497800</v>
+        <v>4356516</v>
       </c>
       <c r="G10" s="29">
-        <v>11778400</v>
-      </c>
-      <c r="H10" s="29">
-        <v>189006200</v>
+        <v>3034340</v>
+      </c>
+      <c r="H10" s="30">
+        <f>D10+E10+F10+G10</f>
+        <v>17446245</v>
       </c>
       <c r="I10" s="30">
+        <f>(B10 + stillbirth*B10/(1000-stillbirth))/(1-abortion)</f>
+        <v>2915890.6635062173</v>
+      </c>
+      <c r="J10" s="105">
+        <f>D10/H10</f>
+        <v>0.22650398409514483</v>
+      </c>
+      <c r="K10" s="30">
         <f t="shared" si="0"/>
-        <v>50520700.000000007</v>
-      </c>
-      <c r="J10" s="30">
-        <f t="shared" si="1"/>
-        <v>3378798.9859621613</v>
-      </c>
-      <c r="K10" s="105">
-        <f t="shared" si="2"/>
-        <v>0.15517797655218554</v>
-      </c>
-      <c r="L10" s="30">
-        <f t="shared" si="3"/>
-        <v>47141901.014037848</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>14530354.336493783</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>2026</v>
       </c>
       <c r="B11" s="8">
-        <v>2836142</v>
+        <v>2530000</v>
       </c>
       <c r="C11" s="29">
-        <v>15709000.000000006</v>
+        <v>11838769</v>
       </c>
       <c r="D11" s="29">
-        <v>7451500.0000000019</v>
+        <v>4065313</v>
       </c>
       <c r="E11" s="29">
-        <v>17944500</v>
+        <v>6319831</v>
       </c>
       <c r="F11" s="29">
-        <v>13426500</v>
+        <v>4477188</v>
       </c>
       <c r="G11" s="29">
-        <v>12168000</v>
-      </c>
-      <c r="H11" s="29">
-        <v>190734000</v>
+        <v>3144612</v>
+      </c>
+      <c r="H11" s="30">
+        <f>D11+E11+F11+G11</f>
+        <v>18006944</v>
       </c>
       <c r="I11" s="30">
+        <f>(B11 + stillbirth*B11/(1000-stillbirth))/(1-abortion)</f>
+        <v>2974678.7817220683</v>
+      </c>
+      <c r="J11" s="105">
+        <f>D11/H11</f>
+        <v>0.22576362763165145</v>
+      </c>
+      <c r="K11" s="30">
         <f t="shared" si="0"/>
-        <v>50990500</v>
-      </c>
-      <c r="J11" s="30">
-        <f t="shared" si="1"/>
-        <v>3344756.3544830228</v>
-      </c>
-      <c r="K11" s="105">
-        <f t="shared" si="2"/>
-        <v>0.1461350643747365</v>
-      </c>
-      <c r="L11" s="30">
-        <f t="shared" si="3"/>
-        <v>47645743.645516977</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>15032265.218277931</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>2027</v>
       </c>
       <c r="B12" s="8">
-        <v>2805541</v>
+        <v>2580000</v>
       </c>
       <c r="C12" s="29">
-        <v>15358200.000000006</v>
+        <v>12092177</v>
       </c>
       <c r="D12" s="29">
-        <v>7411700.0000000019</v>
+        <v>4185562</v>
       </c>
       <c r="E12" s="29">
-        <v>17710400</v>
+        <v>6545116</v>
       </c>
       <c r="F12" s="29">
-        <v>13766300</v>
+        <v>4597739</v>
       </c>
       <c r="G12" s="29">
-        <v>12445000</v>
-      </c>
-      <c r="H12" s="29">
-        <v>192287600</v>
+        <v>3255252</v>
+      </c>
+      <c r="H12" s="30">
+        <f>D12+E12+F12+G12</f>
+        <v>18583669</v>
       </c>
       <c r="I12" s="30">
+        <f>(B12 + stillbirth*B12/(1000-stillbirth))/(1-abortion)</f>
+        <v>3033466.8999379198</v>
+      </c>
+      <c r="J12" s="105">
+        <f>D12/H12</f>
+        <v>0.22522796763114969</v>
+      </c>
+      <c r="K12" s="30">
         <f t="shared" si="0"/>
-        <v>51333400</v>
-      </c>
-      <c r="J12" s="30">
-        <f t="shared" si="1"/>
-        <v>3308667.5799422786</v>
-      </c>
-      <c r="K12" s="105">
-        <f t="shared" si="2"/>
-        <v>0.14438357872262508</v>
-      </c>
-      <c r="L12" s="30">
-        <f t="shared" si="3"/>
-        <v>48024732.420057721</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>15550202.10006208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>2028</v>
       </c>
       <c r="B13" s="8">
-        <v>2773236</v>
+        <v>2630000</v>
       </c>
       <c r="C13" s="29">
-        <v>15007400.000000007</v>
+        <v>12338218</v>
       </c>
       <c r="D13" s="29">
-        <v>7371900.0000000019</v>
+        <v>4309237</v>
       </c>
       <c r="E13" s="29">
-        <v>17476300</v>
+        <v>6776307</v>
       </c>
       <c r="F13" s="29">
-        <v>14106100</v>
+        <v>4722286</v>
       </c>
       <c r="G13" s="29">
-        <v>12722000</v>
-      </c>
-      <c r="H13" s="29">
-        <v>193841200</v>
+        <v>3366750</v>
+      </c>
+      <c r="H13" s="30">
+        <f>D13+E13+F13+G13</f>
+        <v>19174580</v>
       </c>
       <c r="I13" s="30">
+        <f>(B13 + stillbirth*B13/(1000-stillbirth))/(1-abortion)</f>
+        <v>3092255.0181537713</v>
+      </c>
+      <c r="J13" s="105">
+        <f>D13/H13</f>
+        <v>0.22473696946686708</v>
+      </c>
+      <c r="K13" s="30">
         <f t="shared" si="0"/>
-        <v>51676300</v>
-      </c>
-      <c r="J13" s="30">
-        <f t="shared" si="1"/>
-        <v>3270569.2216684073</v>
-      </c>
-      <c r="K13" s="105">
-        <f t="shared" si="2"/>
-        <v>0.14265533716616713</v>
-      </c>
-      <c r="L13" s="30">
-        <f t="shared" si="3"/>
-        <v>48405730.778331593</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>16082324.981846228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>2029</v>
       </c>
       <c r="B14" s="8">
-        <v>2739273</v>
+        <v>2690000</v>
       </c>
       <c r="C14" s="29">
-        <v>14656600.000000007</v>
+        <v>12584924</v>
       </c>
       <c r="D14" s="29">
-        <v>7332100.0000000009</v>
+        <v>4430738</v>
       </c>
       <c r="E14" s="29">
-        <v>17242200</v>
+        <v>7008703</v>
       </c>
       <c r="F14" s="29">
-        <v>14445900</v>
+        <v>4856898</v>
       </c>
       <c r="G14" s="29">
-        <v>12999000</v>
-      </c>
-      <c r="H14" s="29">
-        <v>195394800</v>
+        <v>3479917</v>
+      </c>
+      <c r="H14" s="30">
+        <f>D14+E14+F14+G14</f>
+        <v>19776256</v>
       </c>
       <c r="I14" s="30">
+        <f>(B14 + stillbirth*B14/(1000-stillbirth))/(1-abortion)</f>
+        <v>3162800.7600127924</v>
+      </c>
+      <c r="J14" s="105">
+        <f>D14/H14</f>
+        <v>0.22404331740042199</v>
+      </c>
+      <c r="K14" s="30">
         <f t="shared" si="0"/>
-        <v>52019200</v>
-      </c>
-      <c r="J14" s="30">
-        <f t="shared" si="1"/>
-        <v>3230515.5289875376</v>
-      </c>
-      <c r="K14" s="105">
-        <f t="shared" si="2"/>
-        <v>0.14094988004429135</v>
-      </c>
-      <c r="L14" s="30">
-        <f t="shared" si="3"/>
-        <v>48788684.471012466</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>16613455.239987208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>2030</v>
       </c>
       <c r="B15" s="8">
-        <v>2703670</v>
+        <v>2740000</v>
       </c>
       <c r="C15" s="29">
-        <v>14305800.000000007</v>
+        <v>12839335</v>
       </c>
       <c r="D15" s="29">
-        <v>7292300.0000000009</v>
+        <v>4546624</v>
       </c>
       <c r="E15" s="29">
-        <v>17008100</v>
+        <v>7239465</v>
       </c>
       <c r="F15" s="29">
-        <v>14785700</v>
+        <v>5005361</v>
       </c>
       <c r="G15" s="29">
-        <v>13276000</v>
-      </c>
-      <c r="H15" s="29">
-        <v>196948400</v>
+        <v>3595278</v>
+      </c>
+      <c r="H15" s="30">
+        <f>D15+E15+F15+G15</f>
+        <v>20386728</v>
       </c>
       <c r="I15" s="30">
+        <f>(B15 + stillbirth*B15/(1000-stillbirth))/(1-abortion)</f>
+        <v>3221588.8782286434</v>
+      </c>
+      <c r="J15" s="105">
+        <f>D15/H15</f>
+        <v>0.22301881891002814</v>
+      </c>
+      <c r="K15" s="30">
         <f t="shared" si="0"/>
-        <v>52362100</v>
-      </c>
-      <c r="J15" s="30">
-        <f t="shared" si="1"/>
-        <v>3188527.7298968509</v>
-      </c>
-      <c r="K15" s="105">
-        <f t="shared" si="2"/>
-        <v>0.139266759736527</v>
-      </c>
-      <c r="L15" s="30">
-        <f t="shared" si="3"/>
-        <v>49173572.270103149</v>
+        <v>17165139.121771358</v>
       </c>
     </row>
   </sheetData>
@@ -9204,7 +9057,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -9227,98 +9080,98 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C2" s="49">
         <f>1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE)</f>
-        <v>0.53200836191885958</v>
+        <v>0.54471569980476653</v>
       </c>
       <c r="D2" s="49">
         <f t="shared" ref="D2:G2" si="0">1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE)</f>
-        <v>0.53200836191885958</v>
+        <v>0.54471569980476653</v>
       </c>
       <c r="E2" s="49">
         <f t="shared" si="0"/>
-        <v>0.44274864978114037</v>
+        <v>0.44982829694488635</v>
       </c>
       <c r="F2" s="49">
         <f t="shared" si="0"/>
-        <v>0.24285617786005109</v>
+        <v>0.24457139941017503</v>
       </c>
       <c r="G2" s="49">
         <f t="shared" si="0"/>
-        <v>0.2168920625348294</v>
+        <v>0.23269074767298425</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="49">
         <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5)</f>
-        <v>0.3279916380811404</v>
+        <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="49">
         <f t="shared" ref="D3:G3" si="1">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5)</f>
-        <v>0.3279916380811404</v>
+        <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="49">
         <f t="shared" si="1"/>
-        <v>0.36125135021885962</v>
+        <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="49">
         <f t="shared" si="1"/>
-        <v>0.3761438221399489</v>
+        <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="49">
         <f t="shared" si="1"/>
-        <v>0.36910793746517057</v>
+        <v>0.37372365733745416</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="39">
-        <v>0.10199999999999999</v>
+        <v>8.7000000000000008E-2</v>
       </c>
       <c r="D4" s="39">
-        <v>0.10199999999999999</v>
+        <v>8.7000000000000008E-2</v>
       </c>
       <c r="E4" s="39">
-        <v>0.14699999999999999</v>
+        <v>0.13443032786885245</v>
       </c>
       <c r="F4" s="39">
-        <v>0.247</v>
+        <v>0.24673186710341602</v>
       </c>
       <c r="G4" s="39">
-        <v>0.28100000000000003</v>
+        <v>0.25929610299234518</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="39">
-        <v>3.7999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="D5" s="39">
-        <v>3.7999999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E5" s="39">
-        <v>4.9000000000000002E-2</v>
+        <v>5.6654713114754097E-2</v>
       </c>
       <c r="F5" s="39">
-        <v>0.13400000000000001</v>
+        <v>0.13218483855872717</v>
       </c>
       <c r="G5" s="39">
-        <v>0.13300000000000001</v>
+        <v>0.13428949199721643</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9339,95 +9192,95 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="49">
         <f>1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE)</f>
-        <v>0.43848891822683433</v>
+        <v>0.6241955901533508</v>
       </c>
       <c r="D8" s="49">
         <f t="shared" ref="D8:G8" si="2">1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE)</f>
-        <v>0.43848891822683433</v>
+        <v>0.6241955901533508</v>
       </c>
       <c r="E8" s="49">
         <f t="shared" si="2"/>
-        <v>0.46325746477389407</v>
+        <v>0.68355843805440353</v>
       </c>
       <c r="F8" s="49">
         <f t="shared" si="2"/>
-        <v>0.51282536329943151</v>
+        <v>0.73228840888273117</v>
       </c>
       <c r="G8" s="49">
         <f t="shared" si="2"/>
-        <v>0.55784394006702964</v>
+        <v>0.81212055177975573</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="49">
         <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11)</f>
-        <v>0.36251108177316566</v>
+        <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="49">
         <f t="shared" ref="D9:G9" si="3">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11)</f>
-        <v>0.36251108177316566</v>
+        <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="49">
         <f t="shared" si="3"/>
-        <v>0.35474253522610594</v>
+        <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="49">
         <f t="shared" si="3"/>
-        <v>0.33617463670056846</v>
+        <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="49">
         <f t="shared" si="3"/>
-        <v>0.31615605993297041</v>
+        <v>0.15821429221536368</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="39">
-        <v>0.15</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D10" s="39">
-        <v>0.15</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="E10" s="39">
-        <v>0.129</v>
+        <v>5.4022564102564105E-2</v>
       </c>
       <c r="F10" s="39">
-        <v>0.11</v>
+        <v>4.2547708138447146E-2</v>
       </c>
       <c r="G10" s="39">
-        <v>0.105</v>
+        <v>2.2330660624019519E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" s="39">
-        <v>4.9000000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D11" s="39">
-        <v>4.9000000000000002E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E11" s="39">
-        <v>5.2999999999999999E-2</v>
+        <v>1.5725128205128207E-2</v>
       </c>
       <c r="F11" s="39">
-        <v>4.0999999999999995E-2</v>
+        <v>1.0095416276894293E-2</v>
       </c>
       <c r="G11" s="39">
-        <v>2.1000000000000001E-2</v>
+        <v>7.3344953808610778E-3</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9490,7 +9343,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C14" s="50">
         <v>0.1</v>
@@ -9499,37 +9352,37 @@
         <v>0.1</v>
       </c>
       <c r="E14" s="50">
-        <v>0.74</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="F14" s="50">
-        <v>0.55000000000000004</v>
+        <v>0.72950000000000004</v>
       </c>
       <c r="G14" s="50">
-        <v>0.42699999999999999</v>
+        <v>0.48366666666666674</v>
       </c>
       <c r="H14" s="51">
-        <v>0.48149999999999998</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="I14" s="51">
-        <v>0.48149999999999998</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="J14" s="51">
-        <v>0.48149999999999998</v>
+        <v>0.433</v>
       </c>
       <c r="K14" s="51">
-        <v>0.48149999999999998</v>
+        <v>0.442</v>
       </c>
       <c r="L14" s="51">
-        <v>0.43469999999999998</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="M14" s="51">
-        <v>0.43469999999999998</v>
+        <v>0.44700000000000001</v>
       </c>
       <c r="N14" s="51">
-        <v>0.43469999999999998</v>
+        <v>0.433</v>
       </c>
       <c r="O14" s="51">
-        <v>0.43469999999999998</v>
+        <v>0.442</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9546,47 +9399,47 @@
       </c>
       <c r="E15" s="49">
         <f t="shared" si="4"/>
-        <v>0.31079999999999997</v>
+        <v>0.32801999999999998</v>
       </c>
       <c r="F15" s="49">
         <f t="shared" si="4"/>
-        <v>0.23100000000000001</v>
+        <v>0.30639</v>
       </c>
       <c r="G15" s="49">
         <f t="shared" si="4"/>
-        <v>0.17934</v>
+        <v>0.20314000000000002</v>
       </c>
       <c r="H15" s="49">
         <f t="shared" si="4"/>
-        <v>0.20222999999999999</v>
+        <v>0.19865999999999998</v>
       </c>
       <c r="I15" s="49">
         <f t="shared" si="4"/>
-        <v>0.20222999999999999</v>
+        <v>0.18773999999999999</v>
       </c>
       <c r="J15" s="49">
         <f t="shared" si="4"/>
-        <v>0.20222999999999999</v>
+        <v>0.18185999999999999</v>
       </c>
       <c r="K15" s="49">
         <f t="shared" si="4"/>
-        <v>0.20222999999999999</v>
+        <v>0.18564</v>
       </c>
       <c r="L15" s="49">
         <f t="shared" si="4"/>
-        <v>0.18257399999999999</v>
+        <v>0.19865999999999998</v>
       </c>
       <c r="M15" s="49">
         <f t="shared" si="4"/>
-        <v>0.18257399999999999</v>
+        <v>0.18773999999999999</v>
       </c>
       <c r="N15" s="49">
         <f t="shared" si="4"/>
-        <v>0.18257399999999999</v>
+        <v>0.18185999999999999</v>
       </c>
       <c r="O15" s="49">
         <f t="shared" si="4"/>
-        <v>0.18257399999999999</v>
+        <v>0.18564</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9618,7 +9471,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9629,7 +9482,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -9655,19 +9508,19 @@
         <v>24</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="39">
-        <v>0.80299999999999994</v>
+        <v>0.84</v>
       </c>
       <c r="D2" s="39">
-        <v>0.46200000000000002</v>
+        <v>0.44307448494453255</v>
       </c>
       <c r="E2" s="39">
-        <v>3.3000000000000002E-2</v>
+        <v>1.36244579358196E-2</v>
       </c>
       <c r="F2" s="39">
-        <v>6.9999999999999993E-3</v>
+        <v>0</v>
       </c>
       <c r="G2" s="39">
         <v>0</v>
@@ -9675,19 +9528,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="39">
-        <v>6.8000000000000005E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="D3" s="39">
-        <v>0.16300000000000001</v>
+        <v>0.21674801901743265</v>
       </c>
       <c r="E3" s="39">
-        <v>9.4E-2</v>
+        <v>3.2771032090199478E-2</v>
       </c>
       <c r="F3" s="39">
-        <v>4.4999999999999998E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="G3" s="39">
         <v>0</v>
@@ -9695,19 +9548,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="39">
-        <v>0.107</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D4" s="39">
-        <v>0.37</v>
+        <v>0.31577812995245641</v>
       </c>
       <c r="E4" s="39">
-        <v>0.83700000000000008</v>
+        <v>0.93464267129228107</v>
       </c>
       <c r="F4" s="39">
-        <v>0.879</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="G4" s="39">
         <v>0</v>
@@ -9715,23 +9568,23 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B5" s="67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" s="49">
         <f>1-SUM(C2:C4)</f>
-        <v>2.200000000000002E-2</v>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="D5" s="49">
         <f t="shared" ref="D5:G5" si="0">1-SUM(D2:D4)</f>
-        <v>5.0000000000000044E-3</v>
+        <v>2.4399366085578356E-2</v>
       </c>
       <c r="E5" s="49">
         <f t="shared" si="0"/>
-        <v>3.5999999999999921E-2</v>
+        <v>1.8961838681699872E-2</v>
       </c>
       <c r="F5" s="49">
         <f t="shared" si="0"/>
-        <v>6.899999999999995E-2</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="G5" s="49">
         <f t="shared" si="0"/>
@@ -9762,10 +9615,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -9797,10 +9650,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -9817,10 +9670,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -9837,10 +9690,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -9868,7 +9721,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -9882,10 +9735,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -9899,7 +9752,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -9916,7 +9769,7 @@
         <v>75</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -9930,7 +9783,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B14" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -9956,7 +9809,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9969,35 +9822,37 @@
   <sheetData>
     <row r="1" spans="1:3" s="44" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C1" s="43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="107" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="45">
-        <v>0.15</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="16"/>
       <c r="B3" s="41" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="45">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="16"/>
       <c r="B4" s="41" t="s">
         <v>78</v>
       </c>
@@ -10006,30 +9861,34 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="16"/>
       <c r="B5" s="41" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="45">
-        <v>0.19</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="16"/>
       <c r="B6" s="41" t="s">
         <v>80</v>
       </c>
       <c r="C6" s="45">
-        <v>0.39</v>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="16"/>
       <c r="B7" s="41" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="45">
-        <v>0.19</v>
+        <v>0.29899999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="16"/>
       <c r="B8" s="41" t="s">
         <v>82</v>
       </c>
@@ -10038,59 +9897,65 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="16"/>
       <c r="B9" s="41" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="45">
-        <v>7.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="16"/>
       <c r="B10" s="41" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="45">
-        <v>0.04</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="16"/>
       <c r="B11" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" s="47">
         <f>SUM(C2:C10)</f>
-        <v>0.998</v>
+        <v>1.0010000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="16"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="107" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="41" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="45">
-        <v>0.34</v>
+        <v>0.20799999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="16"/>
       <c r="B14" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="45">
-        <v>0.05</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="16"/>
       <c r="B15" s="41" t="s">
         <v>88</v>
       </c>
       <c r="C15" s="45">
-        <v>7.0000000000000007E-2</v>
+        <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -10098,12 +9963,12 @@
         <v>89</v>
       </c>
       <c r="C16" s="45">
-        <v>0.54</v>
+        <v>0.63700000000000001</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C17" s="47">
         <f>SUM(C13:C16)</f>
@@ -10124,7 +9989,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10137,34 +10002,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="78" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C1" s="79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D1" s="79" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E1" s="79" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="74" t="s">
-        <v>197</v>
-      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
       <c r="E2" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -10176,7 +10037,9 @@
         <v>1</v>
       </c>
       <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
+      <c r="D3" s="74" t="s">
+        <v>196</v>
+      </c>
       <c r="E3" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -10188,7 +10051,9 @@
         <v>2</v>
       </c>
       <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
+      <c r="D4" s="74" t="s">
+        <v>196</v>
+      </c>
       <c r="E4" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -10200,7 +10065,9 @@
         <v>3</v>
       </c>
       <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
+      <c r="D5" s="74" t="s">
+        <v>196</v>
+      </c>
       <c r="E5" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -10212,7 +10079,9 @@
         <v>4</v>
       </c>
       <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="D6" s="74" t="s">
+        <v>196</v>
+      </c>
       <c r="E6" s="97" t="str">
         <f>IF(E$7="","",E$7)</f>
         <v/>
@@ -10221,7 +10090,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="72"/>
       <c r="B7" s="71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" s="70"/>
       <c r="D7" s="69"/>
@@ -10229,7 +10098,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="78" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="77" t="s">
         <v>32</v>
@@ -10238,7 +10107,7 @@
       <c r="D9" s="74"/>
       <c r="E9" s="98" t="str">
         <f>IF(E$14="","",E$14)</f>
-        <v>x</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -10246,16 +10115,9 @@
       <c r="B10" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="74" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" s="97" t="str">
-        <f>IF(E$14="","",E$14)</f>
-        <v>x</v>
-      </c>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="97"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="72"/>
@@ -10264,10 +10126,7 @@
       </c>
       <c r="C11" s="74"/>
       <c r="D11" s="74"/>
-      <c r="E11" s="97" t="str">
-        <f>IF(E$14="","",E$14)</f>
-        <v>x</v>
-      </c>
+      <c r="E11" s="97"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="72"/>
@@ -10276,10 +10135,7 @@
       </c>
       <c r="C12" s="74"/>
       <c r="D12" s="74"/>
-      <c r="E12" s="97" t="str">
-        <f>IF(E$14="","",E$14)</f>
-        <v>x</v>
-      </c>
+      <c r="E12" s="97"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="72"/>
@@ -10288,25 +10144,20 @@
       </c>
       <c r="C13" s="74"/>
       <c r="D13" s="74"/>
-      <c r="E13" s="97" t="str">
-        <f>IF(E$14="","",E$14)</f>
-        <v>x</v>
-      </c>
+      <c r="E13" s="97"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="72"/>
       <c r="B14" s="71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C14" s="70"/>
       <c r="D14" s="69"/>
-      <c r="E14" s="74" t="s">
-        <v>197</v>
-      </c>
+      <c r="E14" s="74"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="76" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" s="71" t="s">
         <v>32</v>
@@ -10369,7 +10220,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="72"/>
       <c r="B21" s="71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C21" s="70"/>
       <c r="D21" s="69"/>
@@ -10390,7 +10241,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10403,16 +10254,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="102" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="103" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="103" t="s">
-        <v>212</v>
-      </c>
       <c r="D1" s="103" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -10423,24 +10274,24 @@
         <v>67</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="103" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3" s="71" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
many changes to facilitate facilitation
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_input.xlsx
+++ b/applications/default/data/national/default_input.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{50E1BEEA-4C3F-3D48-B662-A0DDD12DB3CE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="961" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="12795" windowHeight="15540" tabRatio="961" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -82,12 +76,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -135,12 +129,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{FE58E1C7-CE8A-D54E-AB98-874E3A6FBFD4}">
+    <comment ref="D29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -178,12 +172,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0A00-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,12 +230,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -279,12 +273,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
+    <comment ref="L22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -317,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L24" authorId="0" shapeId="0" xr:uid="{E6EC9594-3F7C-C445-8380-01CE49FD40BB}">
+    <comment ref="L24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -355,13 +349,13 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
     <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -394,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000002000000}">
+    <comment ref="D2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1103,7 +1097,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -3057,8 +3051,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D4020000}"/>
-    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normal 2" xfId="725"/>
+    <cellStyle name="Normal 3" xfId="726"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3099,7 +3093,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3156,7 +3150,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3213,7 +3207,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3270,7 +3264,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3327,7 +3321,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3384,7 +3378,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3441,7 +3435,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3498,7 +3492,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3555,7 +3549,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3612,7 +3606,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3669,7 +3663,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3726,7 +3720,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3783,7 +3777,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3840,7 +3834,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3897,7 +3891,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3954,7 +3948,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4011,7 +4005,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4068,7 +4062,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4117,7 +4111,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4480,7 +4474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -4490,14 +4484,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" style="19" customWidth="1"/>
-    <col min="3" max="16384" width="14.5" style="15"/>
+    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="14.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -4508,12 +4502,12 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>118</v>
       </c>
@@ -4521,7 +4515,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>119</v>
       </c>
@@ -4529,7 +4523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>117</v>
       </c>
@@ -4537,7 +4531,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
         <v>120</v>
       </c>
@@ -4545,7 +4539,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>121</v>
       </c>
@@ -4553,7 +4547,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>122</v>
       </c>
@@ -4561,17 +4555,17 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>106</v>
       </c>
@@ -4579,7 +4573,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>107</v>
       </c>
@@ -4587,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12" t="s">
         <v>108</v>
       </c>
@@ -4595,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12" t="s">
         <v>109</v>
       </c>
@@ -4603,7 +4597,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12" t="s">
         <v>110</v>
       </c>
@@ -4612,15 +4606,15 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="27" t="s">
         <v>113</v>
       </c>
@@ -4628,7 +4622,7 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="27" t="s">
         <v>114</v>
       </c>
@@ -4636,7 +4630,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="27" t="s">
         <v>115</v>
       </c>
@@ -4644,7 +4638,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="27" t="s">
         <v>116</v>
       </c>
@@ -4652,20 +4646,20 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="66" t="s">
         <v>104</v>
       </c>
@@ -4673,7 +4667,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
         <v>103</v>
       </c>
@@ -4683,7 +4677,7 @@
       <c r="D26" s="20"/>
       <c r="E26" s="21"/>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="19" t="s">
         <v>102</v>
       </c>
@@ -4693,7 +4687,7 @@
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
         <v>193</v>
       </c>
@@ -4701,7 +4695,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">
         <v>101</v>
       </c>
@@ -4709,7 +4703,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="66" t="s">
         <v>105</v>
       </c>
@@ -4717,16 +4711,16 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="20"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
         <v>153</v>
       </c>
       <c r="D32" s="20"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="19" t="s">
         <v>9</v>
       </c>
@@ -4735,7 +4729,7 @@
       </c>
       <c r="D33" s="20"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="19" t="s">
         <v>11</v>
       </c>
@@ -4744,7 +4738,7 @@
       </c>
       <c r="D34" s="20"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="19" t="s">
         <v>12</v>
       </c>
@@ -4754,7 +4748,7 @@
       <c r="D35" s="20"/>
       <c r="E35" s="21"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="19" t="s">
         <v>26</v>
       </c>
@@ -4765,16 +4759,16 @@
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D37" s="20"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="20"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="19" t="s">
         <v>142</v>
       </c>
@@ -4783,7 +4777,7 @@
       </c>
       <c r="D39" s="20"/>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="19" t="s">
         <v>143</v>
       </c>
@@ -4791,7 +4785,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="19" t="s">
         <v>144</v>
       </c>
@@ -4799,7 +4793,7 @@
         <v>5.64</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="19" t="s">
         <v>145</v>
       </c>
@@ -4807,7 +4801,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="19" t="s">
         <v>146</v>
       </c>
@@ -4815,12 +4809,12 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="9" t="s">
         <v>123</v>
       </c>
@@ -4828,7 +4822,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="19" t="s">
         <v>151</v>
       </c>
@@ -4836,7 +4830,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="19" t="s">
         <v>155</v>
       </c>
@@ -4844,7 +4838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="19" t="s">
         <v>156</v>
       </c>
@@ -4852,7 +4846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
     </row>
   </sheetData>
@@ -4862,26 +4856,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="56" style="80" customWidth="1"/>
     <col min="2" max="2" width="20" style="59" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="58" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="58" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="58"/>
+    <col min="3" max="3" width="20.42578125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="58" customWidth="1"/>
+    <col min="5" max="16384" width="14.42578125" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="90" t="s">
         <v>70</v>
       </c>
@@ -4895,7 +4889,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="80" t="s">
         <v>29</v>
       </c>
@@ -4909,7 +4903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="80" t="s">
         <v>100</v>
       </c>
@@ -4924,7 +4918,7 @@
       </c>
       <c r="E3" s="87"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="80" t="s">
         <v>97</v>
       </c>
@@ -4939,7 +4933,7 @@
       </c>
       <c r="E4" s="67"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="80" t="s">
         <v>61</v>
       </c>
@@ -4955,7 +4949,7 @@
       </c>
       <c r="E5" s="67"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="80" t="s">
         <v>68</v>
       </c>
@@ -4971,7 +4965,7 @@
       </c>
       <c r="E6" s="86"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="80" t="s">
         <v>63</v>
       </c>
@@ -4986,7 +4980,7 @@
       </c>
       <c r="E7" s="85"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="80" t="s">
         <v>64</v>
       </c>
@@ -5001,7 +4995,7 @@
       </c>
       <c r="E8" s="85"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="80" t="s">
         <v>62</v>
       </c>
@@ -5016,7 +5010,7 @@
       </c>
       <c r="E9" s="85"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="101" t="s">
         <v>217</v>
       </c>
@@ -5030,7 +5024,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="101" t="s">
         <v>218</v>
       </c>
@@ -5044,7 +5038,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="101" t="s">
         <v>219</v>
       </c>
@@ -5058,7 +5052,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="101" t="s">
         <v>220</v>
       </c>
@@ -5072,7 +5066,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>216</v>
       </c>
@@ -5086,7 +5080,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>221</v>
       </c>
@@ -5100,7 +5094,7 @@
         <v>1.78</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="80" t="s">
         <v>57</v>
       </c>
@@ -5115,7 +5109,7 @@
       </c>
       <c r="E16" s="67"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="80" t="s">
         <v>47</v>
       </c>
@@ -5130,7 +5124,7 @@
       </c>
       <c r="E17" s="67"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="80" t="s">
         <v>198</v>
       </c>
@@ -5145,7 +5139,7 @@
         <v>10.49</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="80" t="s">
         <v>197</v>
       </c>
@@ -5160,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="80" t="s">
         <v>195</v>
       </c>
@@ -5175,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="80" t="s">
         <v>158</v>
       </c>
@@ -5190,7 +5184,7 @@
       </c>
       <c r="E21" s="67"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="80" t="s">
         <v>34</v>
       </c>
@@ -5205,7 +5199,7 @@
       </c>
       <c r="E22" s="67"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="80" t="s">
         <v>99</v>
       </c>
@@ -5220,7 +5214,7 @@
       </c>
       <c r="E23" s="67"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="80" t="s">
         <v>98</v>
       </c>
@@ -5235,7 +5229,7 @@
       </c>
       <c r="E24" s="84"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="80" t="s">
         <v>159</v>
       </c>
@@ -5250,7 +5244,7 @@
       </c>
       <c r="E25" s="67"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="80" t="s">
         <v>59</v>
       </c>
@@ -5265,7 +5259,7 @@
       </c>
       <c r="E26" s="67"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="80" t="s">
         <v>95</v>
       </c>
@@ -5279,7 +5273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="80" t="s">
         <v>58</v>
       </c>
@@ -5293,7 +5287,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="80" t="s">
         <v>67</v>
       </c>
@@ -5308,7 +5302,7 @@
         <v>10.015195269175592</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="80" t="s">
         <v>28</v>
       </c>
@@ -5322,7 +5316,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="80" t="s">
         <v>94</v>
       </c>
@@ -5336,7 +5330,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="80" t="s">
         <v>93</v>
       </c>
@@ -5350,7 +5344,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="80" t="s">
         <v>92</v>
       </c>
@@ -5364,7 +5358,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="80" t="s">
         <v>90</v>
       </c>
@@ -5378,7 +5372,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" s="59" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="80" t="s">
         <v>91</v>
       </c>
@@ -5393,7 +5387,7 @@
       </c>
       <c r="F35" s="58"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="80" t="s">
         <v>96</v>
       </c>
@@ -5407,7 +5401,7 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="80" t="s">
         <v>60</v>
       </c>
@@ -5421,7 +5415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F38" s="59"/>
     </row>
   </sheetData>
@@ -5435,7 +5429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5445,13 +5439,13 @@
       <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="91" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="91"/>
+    <col min="1" max="1" width="18.7109375" style="91" customWidth="1"/>
+    <col min="2" max="16384" width="10.85546875" style="91"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A1" s="96" t="s">
         <v>207</v>
       </c>
@@ -5468,7 +5462,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="94" t="s">
         <v>186</v>
       </c>
@@ -5486,7 +5480,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="93"/>
       <c r="B3" s="93" t="s">
         <v>1</v>
@@ -5503,7 +5497,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="93"/>
       <c r="B4" s="93" t="s">
         <v>2</v>
@@ -5520,7 +5514,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="93"/>
       <c r="B5" s="93" t="s">
         <v>3</v>
@@ -5537,7 +5531,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="93"/>
       <c r="B6" s="93" t="s">
         <v>4</v>
@@ -5554,7 +5548,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="92"/>
     </row>
   </sheetData>
@@ -5563,7 +5557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5573,15 +5567,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53" style="80" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="58" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="58"/>
+    <col min="3" max="3" width="42.42578125" style="58" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>70</v>
       </c>
@@ -5592,7 +5586,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>216</v>
       </c>
@@ -5601,7 +5595,7 @@
       </c>
       <c r="C2" s="74"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>221</v>
       </c>
@@ -5610,7 +5604,7 @@
       </c>
       <c r="C3" s="74"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="80" t="s">
         <v>58</v>
       </c>
@@ -5619,7 +5613,7 @@
       </c>
       <c r="C4" s="74"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="80" t="s">
         <v>159</v>
       </c>
@@ -5628,28 +5622,28 @@
       </c>
       <c r="C5" s="74"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
     </row>
   </sheetData>
@@ -5660,7 +5654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5670,85 +5664,85 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" style="58" customWidth="1"/>
-    <col min="2" max="16384" width="11.5" style="58"/>
+    <col min="1" max="1" width="30.140625" style="58" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="74" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="74" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="74" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="74" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="74" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="74" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="74" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="74"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="74"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="74"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="74"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="74"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="74"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="74"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="74"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="74"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="74"/>
     </row>
   </sheetData>
@@ -5758,7 +5752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -5768,9 +5762,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -5790,7 +5784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
@@ -5815,7 +5809,7 @@
         <v>1.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -5840,7 +5834,7 @@
         <v>5.8059717622450747E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
@@ -5873,7 +5867,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5883,19 +5877,19 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5942,7 +5936,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -5993,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>171</v>
       </c>
@@ -6037,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>158</v>
       </c>
@@ -6083,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>159</v>
       </c>
@@ -6130,7 +6124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="52" t="s">
         <v>95</v>
       </c>
@@ -6174,7 +6168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>58</v>
       </c>
@@ -6220,7 +6214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
         <v>67</v>
       </c>
@@ -6268,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="14" t="s">
         <v>28</v>
       </c>
@@ -6312,7 +6306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="52" t="s">
         <v>96</v>
       </c>
@@ -6356,7 +6350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
         <v>60</v>
       </c>
@@ -6400,10 +6394,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="52"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -6454,7 +6448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="14" t="s">
         <v>97</v>
@@ -6499,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="14" t="s">
         <v>216</v>
@@ -6548,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="14" t="s">
         <v>221</v>
@@ -6597,7 +6591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="52" t="s">
         <v>57</v>
       </c>
@@ -6645,7 +6639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
         <v>99</v>
       </c>
@@ -6689,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>98</v>
       </c>
@@ -6733,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="52" t="s">
         <v>59</v>
       </c>
@@ -6781,10 +6775,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="52"/>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="99" t="s">
         <v>37</v>
       </c>
@@ -6831,7 +6825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="101" t="s">
         <v>68</v>
       </c>
@@ -6875,7 +6869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="101" t="s">
         <v>217</v>
       </c>
@@ -6923,7 +6917,7 @@
         <v>0.54921999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="101" t="s">
         <v>218</v>
       </c>
@@ -6971,7 +6965,7 @@
         <v>0.23537999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="101" t="s">
         <v>219</v>
       </c>
@@ -7019,7 +7013,7 @@
         <v>0.21539999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="101" t="s">
         <v>220</v>
       </c>
@@ -7064,7 +7058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="14"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -7074,7 +7068,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -7132,7 +7126,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="14" t="s">
         <v>64</v>
       </c>
@@ -7187,7 +7181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
@@ -7242,7 +7236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="14" t="s">
         <v>47</v>
       </c>
@@ -7286,7 +7280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="14" t="s">
         <v>34</v>
       </c>
@@ -7343,7 +7337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="52" t="s">
         <v>94</v>
       </c>
@@ -7387,7 +7381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="52" t="s">
         <v>93</v>
@@ -7432,7 +7426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="52" t="s">
         <v>92</v>
       </c>
@@ -7476,7 +7470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="52" t="s">
         <v>90</v>
       </c>
@@ -7520,7 +7514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="52" t="s">
         <v>91</v>
       </c>
@@ -7564,7 +7558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="52"/>
     </row>
   </sheetData>
@@ -7578,7 +7572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -7588,16 +7582,16 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="58" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="58" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="58"/>
-    <col min="5" max="5" width="17.5" style="58" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="58"/>
+    <col min="1" max="1" width="33.7109375" style="58" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="58" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="58"/>
+    <col min="5" max="5" width="17.42578125" style="58" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>185</v>
       </c>
@@ -7614,7 +7608,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="62" t="s">
         <v>180</v>
       </c>
@@ -7632,7 +7626,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="62" t="s">
         <v>179</v>
       </c>
@@ -7650,7 +7644,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="62" t="s">
         <v>178</v>
       </c>
@@ -7668,7 +7662,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="62" t="s">
         <v>177</v>
       </c>
@@ -7686,7 +7680,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="62" t="s">
         <v>176</v>
       </c>
@@ -7704,7 +7698,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="62" t="s">
         <v>175</v>
       </c>
@@ -7722,7 +7716,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="62" t="s">
         <v>174</v>
       </c>
@@ -7740,7 +7734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="62" t="s">
         <v>173</v>
       </c>
@@ -7758,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="62" t="s">
         <v>172</v>
       </c>
@@ -7776,7 +7770,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="59"/>
     </row>
   </sheetData>
@@ -7787,7 +7781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -7797,13 +7791,13 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>127</v>
       </c>
@@ -7826,7 +7820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>74</v>
       </c>
@@ -7849,7 +7843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
@@ -7872,7 +7866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
@@ -7895,7 +7889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>10</v>
       </c>
@@ -7918,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -7941,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -7964,7 +7958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>27</v>
       </c>
@@ -7987,7 +7981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>15</v>
       </c>
@@ -8010,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>72</v>
       </c>
@@ -8033,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -8056,7 +8050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
@@ -8079,7 +8073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>18</v>
       </c>
@@ -8102,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
@@ -8125,7 +8119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -8148,7 +8142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>21</v>
       </c>
@@ -8171,7 +8165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>22</v>
       </c>
@@ -8194,7 +8188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>23</v>
       </c>
@@ -8217,7 +8211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>38</v>
       </c>
@@ -8240,7 +8234,7 @@
         <v>0.10082724000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>39</v>
       </c>
@@ -8263,7 +8257,7 @@
         <v>3.1206000000000002E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>40</v>
       </c>
@@ -8286,7 +8280,7 @@
         <v>0.15891214000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
@@ -8309,7 +8303,7 @@
         <v>0.12598688999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -8332,7 +8326,7 @@
         <v>0.12434007</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>43</v>
       </c>
@@ -8355,7 +8349,7 @@
         <v>3.9028409999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>44</v>
       </c>
@@ -8378,7 +8372,7 @@
         <v>8.5254999999999999E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>45</v>
       </c>
@@ -8401,7 +8395,7 @@
         <v>6.8467810000000004E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>46</v>
       </c>
@@ -8432,7 +8426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -8442,16 +8436,16 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="15" customWidth="1"/>
-    <col min="2" max="9" width="16.83203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" style="15" customWidth="1"/>
-    <col min="12" max="16384" width="14.5" style="15"/>
+    <col min="1" max="1" width="8.42578125" style="15" customWidth="1"/>
+    <col min="2" max="9" width="16.85546875" style="15" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="14.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
@@ -8486,7 +8480,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>2017</v>
       </c>
@@ -8509,15 +8503,15 @@
         <v>2174712</v>
       </c>
       <c r="H2" s="30">
-        <f>D2+E2+F2+G2</f>
+        <f t="shared" ref="H2:H15" si="0">D2+E2+F2+G2</f>
         <v>13370081</v>
       </c>
       <c r="I2" s="30">
-        <f>(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" ref="I2:I15" si="1">(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
         <v>2480858.588708919</v>
       </c>
       <c r="J2" s="105">
-        <f>D2/H2</f>
+        <f t="shared" ref="J2:J15" si="2">D2/H2</f>
         <v>0.22677775848927167</v>
       </c>
       <c r="K2" s="30">
@@ -8525,7 +8519,7 @@
         <v>10889222.411291081</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>2018</v>
       </c>
@@ -8548,23 +8542,23 @@
         <v>2275309</v>
       </c>
       <c r="H3" s="30">
-        <f>D3+E3+F3+G3</f>
+        <f t="shared" si="0"/>
         <v>13842766</v>
       </c>
       <c r="I3" s="30">
-        <f>(B3 + stillbirth*B3/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2527889.0832815999</v>
       </c>
       <c r="J3" s="105">
-        <f>D3/H3</f>
+        <f t="shared" si="2"/>
         <v>0.22861572607671038</v>
       </c>
       <c r="K3" s="30">
-        <f t="shared" ref="K3:K15" si="0">H3-I3</f>
+        <f t="shared" ref="K3:K15" si="3">H3-I3</f>
         <v>11314876.916718401</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>2019</v>
       </c>
@@ -8587,23 +8581,23 @@
         <v>2379017</v>
       </c>
       <c r="H4" s="30">
-        <f>D4+E4+F4+G4</f>
+        <f t="shared" si="0"/>
         <v>14328740</v>
       </c>
       <c r="I4" s="30">
-        <f>(B4 + stillbirth*B4/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2586677.2014974509</v>
       </c>
       <c r="J4" s="105">
-        <f>D4/H4</f>
+        <f t="shared" si="2"/>
         <v>0.23005190965849057</v>
       </c>
       <c r="K4" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>11742062.79850255</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>2020</v>
       </c>
@@ -8626,23 +8620,23 @@
         <v>2484409</v>
       </c>
       <c r="H5" s="30">
-        <f>D5+E5+F5+G5</f>
+        <f t="shared" si="0"/>
         <v>14821716</v>
       </c>
       <c r="I5" s="30">
-        <f>(B5 + stillbirth*B5/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2633707.6960701318</v>
       </c>
       <c r="J5" s="105">
-        <f>D5/H5</f>
+        <f t="shared" si="2"/>
         <v>0.23067295311824892</v>
       </c>
       <c r="K5" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12188008.303929869</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>2021</v>
       </c>
@@ -8665,23 +8659,23 @@
         <v>2592003</v>
       </c>
       <c r="H6" s="30">
-        <f>D6+E6+F6+G6</f>
+        <f t="shared" si="0"/>
         <v>15326652</v>
       </c>
       <c r="I6" s="30">
-        <f>(B6 + stillbirth*B6/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2680738.1906428128</v>
       </c>
       <c r="J6" s="105">
-        <f>D6/H6</f>
+        <f t="shared" si="2"/>
         <v>0.23049769773594389</v>
       </c>
       <c r="K6" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>12645913.809357187</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>2022</v>
       </c>
@@ -8704,23 +8698,23 @@
         <v>2701259</v>
       </c>
       <c r="H7" s="30">
-        <f>D7+E7+F7+G7</f>
+        <f t="shared" si="0"/>
         <v>15838161</v>
       </c>
       <c r="I7" s="30">
-        <f>(B7 + stillbirth*B7/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2739526.3088586638</v>
       </c>
       <c r="J7" s="105">
-        <f>D7/H7</f>
+        <f t="shared" si="2"/>
         <v>0.22965987023367171</v>
       </c>
       <c r="K7" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>13098634.691141337</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>2023</v>
       </c>
@@ -8743,23 +8737,23 @@
         <v>2811667</v>
       </c>
       <c r="H8" s="30">
-        <f>D8+E8+F8+G8</f>
+        <f t="shared" si="0"/>
         <v>16358958</v>
       </c>
       <c r="I8" s="30">
-        <f>(B8 + stillbirth*B8/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2798314.4270745148</v>
       </c>
       <c r="J8" s="105">
-        <f>D8/H8</f>
+        <f t="shared" si="2"/>
         <v>0.22846216733364069</v>
       </c>
       <c r="K8" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>13560643.572925486</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>2024</v>
       </c>
@@ -8782,23 +8776,23 @@
         <v>2922818</v>
       </c>
       <c r="H9" s="30">
-        <f>D9+E9+F9+G9</f>
+        <f t="shared" si="0"/>
         <v>16894224</v>
       </c>
       <c r="I9" s="30">
-        <f>(B9 + stillbirth*B9/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2845344.9216471957</v>
       </c>
       <c r="J9" s="105">
-        <f>D9/H9</f>
+        <f t="shared" si="2"/>
         <v>0.22733651453893355</v>
       </c>
       <c r="K9" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14048879.078352805</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>2025</v>
       </c>
@@ -8821,23 +8815,23 @@
         <v>3034340</v>
       </c>
       <c r="H10" s="30">
-        <f>D10+E10+F10+G10</f>
+        <f t="shared" si="0"/>
         <v>17446245</v>
       </c>
       <c r="I10" s="30">
-        <f>(B10 + stillbirth*B10/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2915890.6635062173</v>
       </c>
       <c r="J10" s="105">
-        <f>D10/H10</f>
+        <f t="shared" si="2"/>
         <v>0.22650398409514483</v>
       </c>
       <c r="K10" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>14530354.336493783</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>2026</v>
       </c>
@@ -8860,23 +8854,23 @@
         <v>3144612</v>
       </c>
       <c r="H11" s="30">
-        <f>D11+E11+F11+G11</f>
+        <f t="shared" si="0"/>
         <v>18006944</v>
       </c>
       <c r="I11" s="30">
-        <f>(B11 + stillbirth*B11/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>2974678.7817220683</v>
       </c>
       <c r="J11" s="105">
-        <f>D11/H11</f>
+        <f t="shared" si="2"/>
         <v>0.22576362763165145</v>
       </c>
       <c r="K11" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15032265.218277931</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>2027</v>
       </c>
@@ -8899,23 +8893,23 @@
         <v>3255252</v>
       </c>
       <c r="H12" s="30">
-        <f>D12+E12+F12+G12</f>
+        <f t="shared" si="0"/>
         <v>18583669</v>
       </c>
       <c r="I12" s="30">
-        <f>(B12 + stillbirth*B12/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>3033466.8999379198</v>
       </c>
       <c r="J12" s="105">
-        <f>D12/H12</f>
+        <f t="shared" si="2"/>
         <v>0.22522796763114969</v>
       </c>
       <c r="K12" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>15550202.10006208</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>2028</v>
       </c>
@@ -8938,23 +8932,23 @@
         <v>3366750</v>
       </c>
       <c r="H13" s="30">
-        <f>D13+E13+F13+G13</f>
+        <f t="shared" si="0"/>
         <v>19174580</v>
       </c>
       <c r="I13" s="30">
-        <f>(B13 + stillbirth*B13/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>3092255.0181537713</v>
       </c>
       <c r="J13" s="105">
-        <f>D13/H13</f>
+        <f t="shared" si="2"/>
         <v>0.22473696946686708</v>
       </c>
       <c r="K13" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16082324.981846228</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>2029</v>
       </c>
@@ -8977,23 +8971,23 @@
         <v>3479917</v>
       </c>
       <c r="H14" s="30">
-        <f>D14+E14+F14+G14</f>
+        <f t="shared" si="0"/>
         <v>19776256</v>
       </c>
       <c r="I14" s="30">
-        <f>(B14 + stillbirth*B14/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>3162800.7600127924</v>
       </c>
       <c r="J14" s="105">
-        <f>D14/H14</f>
+        <f t="shared" si="2"/>
         <v>0.22404331740042199</v>
       </c>
       <c r="K14" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16613455.239987208</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>2030</v>
       </c>
@@ -9016,19 +9010,19 @@
         <v>3595278</v>
       </c>
       <c r="H15" s="30">
-        <f>D15+E15+F15+G15</f>
+        <f t="shared" si="0"/>
         <v>20386728</v>
       </c>
       <c r="I15" s="30">
-        <f>(B15 + stillbirth*B15/(1000-stillbirth))/(1-abortion)</f>
+        <f t="shared" si="1"/>
         <v>3221588.8782286434</v>
       </c>
       <c r="J15" s="105">
-        <f>D15/H15</f>
+        <f t="shared" si="2"/>
         <v>0.22301881891002814</v>
       </c>
       <c r="K15" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>17165139.121771358</v>
       </c>
     </row>
@@ -9039,7 +9033,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9049,13 +9043,13 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>152</v>
       </c>
@@ -9078,7 +9072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>130</v>
       </c>
@@ -9106,17 +9100,17 @@
         <v>0.23269074767298425</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="14" t="s">
         <v>133</v>
       </c>
       <c r="C3" s="49">
-        <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5)</f>
+        <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5)</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="49">
-        <f t="shared" ref="D3:G3" si="1">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5)</f>
+        <f t="shared" ref="D3:G3" si="1">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5)</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="49">
@@ -9132,7 +9126,7 @@
         <v>0.37372365733745416</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="14" t="s">
         <v>131</v>
@@ -9153,7 +9147,7 @@
         <v>0.25929610299234518</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="14" t="s">
         <v>134</v>
@@ -9174,7 +9168,7 @@
         <v>0.13428949199721643</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="17"/>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -9182,7 +9176,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -9190,7 +9184,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>129</v>
       </c>
@@ -9218,16 +9212,16 @@
         <v>0.81212055177975573</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>136</v>
       </c>
       <c r="C9" s="49">
-        <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11)</f>
+        <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11)</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="49">
-        <f t="shared" ref="D9:G9" si="3">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11)</f>
+        <f t="shared" ref="D9:G9" si="3">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11)</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="49">
@@ -9243,7 +9237,7 @@
         <v>0.15821429221536368</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>137</v>
       </c>
@@ -9263,7 +9257,7 @@
         <v>2.2330660624019519E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>138</v>
       </c>
@@ -9283,7 +9277,7 @@
         <v>7.3344953808610778E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -9297,7 +9291,7 @@
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
     </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>71</v>
       </c>
@@ -9341,7 +9335,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>150</v>
       </c>
@@ -9385,7 +9379,7 @@
         <v>0.442</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>69</v>
       </c>
@@ -9442,14 +9436,14 @@
         <v>0.18564</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -9464,7 +9458,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9474,13 +9468,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="7" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
         <v>128</v>
       </c>
@@ -9503,7 +9497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -9526,7 +9520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="67" t="s">
         <v>189</v>
       </c>
@@ -9546,7 +9540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="67" t="s">
         <v>190</v>
       </c>
@@ -9566,7 +9560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="67" t="s">
         <v>191</v>
       </c>
@@ -9597,7 +9591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9607,13 +9601,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>160</v>
       </c>
@@ -9648,7 +9642,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -9665,10 +9659,10 @@
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -9685,10 +9679,10 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -9705,7 +9699,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -9719,7 +9713,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>166</v>
       </c>
@@ -9733,7 +9727,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -9750,7 +9744,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="53" t="s">
         <v>168</v>
       </c>
@@ -9764,7 +9758,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>75</v>
       </c>
@@ -9781,7 +9775,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>192</v>
       </c>
@@ -9802,7 +9796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -9812,15 +9806,15 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="15"/>
+    <col min="1" max="1" width="37.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="44" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="44" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>141</v>
       </c>
@@ -9831,7 +9825,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="107" t="s">
         <v>140</v>
       </c>
@@ -9842,7 +9836,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
       <c r="B3" s="41" t="s">
         <v>77</v>
@@ -9851,7 +9845,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="41" t="s">
         <v>78</v>
@@ -9860,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="41" t="s">
         <v>79</v>
@@ -9869,7 +9863,7 @@
         <v>0.152</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="41" t="s">
         <v>80</v>
@@ -9878,7 +9872,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="41" t="s">
         <v>81</v>
@@ -9887,7 +9881,7 @@
         <v>0.29899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="41" t="s">
         <v>82</v>
@@ -9896,7 +9890,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="41" t="s">
         <v>83</v>
@@ -9905,7 +9899,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="41" t="s">
         <v>84</v>
@@ -9914,7 +9908,7 @@
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="48" t="s">
         <v>147</v>
@@ -9924,12 +9918,12 @@
         <v>1.0010000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="107" t="s">
         <v>85</v>
       </c>
@@ -9940,7 +9934,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="41" t="s">
         <v>87</v>
@@ -9949,7 +9943,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="41" t="s">
         <v>88</v>
@@ -9958,7 +9952,7 @@
         <v>0.11899999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="41" t="s">
         <v>89</v>
       </c>
@@ -9966,7 +9960,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="48" t="s">
         <v>147</v>
       </c>
@@ -9982,7 +9976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9992,15 +9986,15 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="58" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="58" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="58" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="58"/>
+    <col min="2" max="2" width="19.140625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="58" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
         <v>203</v>
       </c>
@@ -10017,7 +10011,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="76" t="s">
         <v>198</v>
       </c>
@@ -10031,7 +10025,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="72"/>
       <c r="B3" s="71" t="s">
         <v>1</v>
@@ -10045,7 +10039,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="72"/>
       <c r="B4" s="71" t="s">
         <v>2</v>
@@ -10059,7 +10053,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="72"/>
       <c r="B5" s="71" t="s">
         <v>3</v>
@@ -10073,7 +10067,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="72"/>
       <c r="B6" s="71" t="s">
         <v>4</v>
@@ -10087,7 +10081,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="72"/>
       <c r="B7" s="71" t="s">
         <v>194</v>
@@ -10096,7 +10090,7 @@
       <c r="D7" s="69"/>
       <c r="E7" s="74"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="78" t="s">
         <v>197</v>
       </c>
@@ -10110,7 +10104,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="72"/>
       <c r="B10" s="71" t="s">
         <v>1</v>
@@ -10119,7 +10113,7 @@
       <c r="D10" s="74"/>
       <c r="E10" s="97"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="72"/>
       <c r="B11" s="71" t="s">
         <v>2</v>
@@ -10128,7 +10122,7 @@
       <c r="D11" s="74"/>
       <c r="E11" s="97"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="72"/>
       <c r="B12" s="71" t="s">
         <v>3</v>
@@ -10137,7 +10131,7 @@
       <c r="D12" s="74"/>
       <c r="E12" s="97"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="72"/>
       <c r="B13" s="71" t="s">
         <v>4</v>
@@ -10146,7 +10140,7 @@
       <c r="D13" s="74"/>
       <c r="E13" s="97"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="72"/>
       <c r="B14" s="71" t="s">
         <v>194</v>
@@ -10155,7 +10149,7 @@
       <c r="D14" s="69"/>
       <c r="E14" s="74"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="76" t="s">
         <v>195</v>
       </c>
@@ -10169,7 +10163,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="72"/>
       <c r="B17" s="71" t="s">
         <v>1</v>
@@ -10181,7 +10175,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="72"/>
       <c r="B18" s="71" t="s">
         <v>2</v>
@@ -10193,7 +10187,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="72"/>
       <c r="B19" s="71" t="s">
         <v>3</v>
@@ -10205,7 +10199,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="72"/>
       <c r="B20" s="71" t="s">
         <v>4</v>
@@ -10217,7 +10211,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="72"/>
       <c r="B21" s="71" t="s">
         <v>194</v>
@@ -10234,7 +10228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE4650B-7A35-4B48-AEF2-692F4EBB38C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10244,15 +10238,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="102" t="s">
         <v>186</v>
       </c>
@@ -10266,7 +10260,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="103" t="s">
         <v>70</v>
       </c>
@@ -10280,7 +10274,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="103" t="s">
         <v>214</v>
       </c>

</xml_diff>

<commit_message>
Removed IFA fort of rice, wheat for demo
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_input.xlsx
+++ b/applications/default/data/national/default_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8FA8780D-B6E0-314E-936E-040797774EA5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9D614775-B75F-3549-9198-F5DFF0A8E1AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="219">
   <si>
     <t>year</t>
   </si>
@@ -4720,10 +4720,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4810,7 +4810,7 @@
       </c>
       <c r="E5" s="80"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="74" t="s">
         <v>63</v>
       </c>
@@ -4826,8 +4826,8 @@
       <c r="E6" s="79"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="74" t="s">
-        <v>64</v>
+      <c r="A7" s="93" t="s">
+        <v>214</v>
       </c>
       <c r="B7" s="75">
         <v>0</v>
@@ -4836,13 +4836,12 @@
         <v>0.95</v>
       </c>
       <c r="D7" s="76">
-        <v>0.75</v>
-      </c>
-      <c r="E7" s="79"/>
+        <v>0.73</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="74" t="s">
-        <v>62</v>
+      <c r="A8" s="93" t="s">
+        <v>215</v>
       </c>
       <c r="B8" s="75">
         <v>0</v>
@@ -4851,13 +4850,12 @@
         <v>0.95</v>
       </c>
       <c r="D8" s="76">
-        <v>0.19</v>
-      </c>
-      <c r="E8" s="79"/>
+        <v>1.78</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="93" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B9" s="75">
         <v>0</v>
@@ -4866,12 +4864,12 @@
         <v>0.95</v>
       </c>
       <c r="D9" s="76">
-        <v>0.73</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="93" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B10" s="75">
         <v>0</v>
@@ -4880,12 +4878,12 @@
         <v>0.95</v>
       </c>
       <c r="D10" s="76">
-        <v>1.78</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="93" t="s">
-        <v>216</v>
+      <c r="A11" s="14" t="s">
+        <v>213</v>
       </c>
       <c r="B11" s="75">
         <v>0</v>
@@ -4894,12 +4892,12 @@
         <v>0.95</v>
       </c>
       <c r="D11" s="76">
-        <v>0.24</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="93" t="s">
-        <v>217</v>
+      <c r="A12" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="B12" s="75">
         <v>0</v>
@@ -4908,85 +4906,87 @@
         <v>0.95</v>
       </c>
       <c r="D12" s="76">
-        <v>0.55000000000000004</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14" t="s">
-        <v>213</v>
+      <c r="A13" s="74" t="s">
+        <v>57</v>
       </c>
       <c r="B13" s="75">
-        <v>0</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="C13" s="75">
         <v>0.95</v>
       </c>
       <c r="D13" s="76">
-        <v>0.73</v>
-      </c>
+        <v>2.06</v>
+      </c>
+      <c r="E13" s="65"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="14" t="s">
-        <v>218</v>
+      <c r="A14" s="74" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="75">
-        <v>0</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="C14" s="75">
         <v>0.95</v>
       </c>
       <c r="D14" s="76">
-        <v>1.78</v>
-      </c>
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="65"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="74" t="s">
-        <v>57</v>
+        <v>195</v>
       </c>
       <c r="B15" s="75">
-        <v>0.34599999999999997</v>
+        <v>0</v>
       </c>
       <c r="C15" s="75">
         <v>0.95</v>
       </c>
-      <c r="D15" s="76">
-        <v>2.06</v>
-      </c>
-      <c r="E15" s="65"/>
+      <c r="D15" s="92">
+        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
+        <v>10.49</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="74" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="B16" s="75">
-        <v>0.80800000000000005</v>
+        <v>0</v>
       </c>
       <c r="C16" s="75">
         <v>0.95</v>
       </c>
       <c r="D16" s="76">
-        <v>0.05</v>
+        <v>50</v>
       </c>
       <c r="E16" s="65"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="74" t="s">
-        <v>195</v>
+        <v>34</v>
       </c>
       <c r="B17" s="75">
-        <v>0</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="C17" s="75">
         <v>0.95</v>
       </c>
-      <c r="D17" s="92">
-        <f>SUMPRODUCT(('IYCF cost'!$C$2:$E$6)*('IYCF packages'!$C$2:$E$6&lt;&gt;""))</f>
-        <v>10.49</v>
-      </c>
+      <c r="D17" s="76">
+        <v>2.61</v>
+      </c>
+      <c r="E17" s="65"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="74" t="s">
-        <v>157</v>
+        <v>99</v>
       </c>
       <c r="B18" s="75">
         <v>0</v>
@@ -4995,88 +4995,86 @@
         <v>0.95</v>
       </c>
       <c r="D18" s="76">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E18" s="65"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="74" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="B19" s="75">
-        <v>0.50800000000000001</v>
+        <v>0</v>
       </c>
       <c r="C19" s="75">
         <v>0.95</v>
       </c>
       <c r="D19" s="76">
-        <v>2.61</v>
-      </c>
-      <c r="E19" s="65"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="78"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="74" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="B20" s="75">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C20" s="75">
         <v>0.95</v>
       </c>
       <c r="D20" s="76">
-        <v>1</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="74" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="B21" s="75">
-        <v>0</v>
+        <v>0.3538</v>
       </c>
       <c r="C21" s="75">
         <v>0.95</v>
       </c>
       <c r="D21" s="76">
-        <v>1</v>
-      </c>
-      <c r="E21" s="78"/>
+        <v>3.78</v>
+      </c>
+      <c r="E21" s="65"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="74" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="B22" s="75">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="75">
         <v>0.95</v>
       </c>
       <c r="D22" s="76">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="E22" s="65"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="75">
-        <v>0.3538</v>
+        <v>0</v>
       </c>
       <c r="C23" s="75">
         <v>0.95</v>
       </c>
       <c r="D23" s="76">
-        <v>3.78</v>
-      </c>
-      <c r="E23" s="65"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="74" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B24" s="75">
         <v>0</v>
@@ -5084,158 +5082,130 @@
       <c r="C24" s="75">
         <v>0.95</v>
       </c>
-      <c r="D24" s="76">
-        <v>1</v>
+      <c r="D24" s="77">
+        <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
+        <v>10.015195269175592</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="74" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="B25" s="75">
-        <v>0</v>
+        <v>0.89970000000000006</v>
       </c>
       <c r="C25" s="75">
         <v>0.95</v>
       </c>
       <c r="D25" s="76">
-        <v>48</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="74" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="B26" s="75">
-        <v>0</v>
+        <v>0.80700000000000005</v>
       </c>
       <c r="C26" s="75">
         <v>0.95</v>
       </c>
-      <c r="D26" s="77">
-        <f>90*AVERAGE('Incidence of conditions'!B4:F4) + 40*AVERAGE('Incidence of conditions'!B3:F3)*IF(ISBLANK(manage_mam), 0, 1)</f>
-        <v>10.015195269175592</v>
+      <c r="D26" s="76">
+        <v>0.9</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="74" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="B27" s="75">
-        <v>0.89970000000000006</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="C27" s="75">
         <v>0.95</v>
       </c>
       <c r="D27" s="76">
-        <v>0.41</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B28" s="75">
-        <v>0.80700000000000005</v>
+        <v>0.316</v>
       </c>
       <c r="C28" s="75">
         <v>0.95</v>
       </c>
       <c r="D28" s="76">
-        <v>0.9</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="74" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B29" s="75">
-        <v>0.73199999999999998</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="C29" s="75">
         <v>0.95</v>
       </c>
       <c r="D29" s="76">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B30" s="75">
-        <v>0.316</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="C30" s="75">
         <v>0.95</v>
       </c>
       <c r="D30" s="76">
-        <v>79</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F30" s="56"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="74" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B31" s="75">
-        <v>0.59699999999999998</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="C31" s="75">
         <v>0.95</v>
       </c>
       <c r="D31" s="76">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="74" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="B32" s="75">
-        <v>0.19900000000000001</v>
+        <v>0</v>
       </c>
       <c r="C32" s="75">
         <v>0.95</v>
       </c>
       <c r="D32" s="76">
-        <v>102</v>
-      </c>
-      <c r="F32" s="56"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="74" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="75">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="C33" s="75">
-        <v>0.95</v>
-      </c>
-      <c r="D33" s="76">
-        <v>5.53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="75">
-        <v>0</v>
-      </c>
-      <c r="C34" s="75">
-        <v>0.95</v>
-      </c>
-      <c r="D34" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F35" s="57"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F33" s="57"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D34">
-    <sortCondition ref="A2:A34"/>
+  <sortState ref="A2:D32">
+    <sortCondition ref="A2:A32"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9571,8 +9541,8 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Couple updates to demo spreadsheets
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_input.xlsx
+++ b/applications/default/data/national/default_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9D614775-B75F-3549-9198-F5DFF0A8E1AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ABD6EA5A-CCC5-3B47-A3EF-7DE2397E9CDA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -87,59 +87,6 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-If user wants this, it must be checked for </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>all populations</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> b/c they are all targetted at once.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
         <r>
@@ -192,7 +139,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -235,7 +182,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -1154,7 +1101,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1164,12 +1111,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1990,7 +1931,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2043,7 +1984,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="9" fillId="4" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2051,7 +1992,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2061,7 +2002,7 @@
     <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="4" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2070,7 +2011,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2098,13 +2039,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="4" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2115,10 +2056,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
@@ -2137,8 +2078,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2152,7 +2093,7 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
@@ -2169,9 +2110,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="4" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="25" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2181,7 +2122,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4341,7 +4281,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4379,7 +4319,7 @@
       <c r="B4" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="98">
+      <c r="C4" s="23">
         <v>1</v>
       </c>
     </row>
@@ -4722,7 +4662,7 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -9565,7 +9505,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="98" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="41" t="s">
@@ -9663,7 +9603,7 @@
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="98" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="41" t="s">
@@ -9715,14 +9655,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9832,7 +9772,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed cost of IFA
</commit_message>
<xml_diff>
--- a/applications/default/data/national/default_input.xlsx
+++ b/applications/default/data/national/default_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/default/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{ABD6EA5A-CCC5-3B47-A3EF-7DE2397E9CDA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A94EA66-2917-5343-A3D5-7B728357D7E7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4662,8 +4662,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4761,7 +4761,7 @@
         <v>0.95</v>
       </c>
       <c r="D6" s="76">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="E6" s="79"/>
     </row>
@@ -9661,7 +9661,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>